<commit_message>
Upload Toplevel and Atmos (some parts are still missing) for NICAM16-9s, turn "on" to publish.
</commit_message>
<xml_diff>
--- a/cmip6/models/nicam16-9s/cmip6_miroc_nicam16-9s_atmos.xlsx
+++ b/cmip6/models/nicam16-9s/cmip6_miroc_nicam16-9s_atmos.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\kodama_home\研究\CMIP\CMIP6\ES-DOC\03.とりまとめ\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C4DB9E-5908-4155-90E8-09B1B276535F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="14616" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" r:id="rId1"/>
@@ -20,12 +26,12 @@
     <sheet name="9. Gravity Waves" sheetId="11" r:id="rId11"/>
     <sheet name="10. Natural Forcing" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1606" uniqueCount="1083">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1672" uniqueCount="1105">
   <si>
     <t>ES-DOC CMIP6 Model Documentation</t>
   </si>
@@ -3274,17 +3280,104 @@
   </si>
   <si>
     <t>Stratospheric aerosols optical thickness</t>
+  </si>
+  <si>
+    <t>Improved Mellor-Yamada level 2 scheme, MYNN (Nakanishi and Niino 2006, JMSJ)</t>
+  </si>
+  <si>
+    <t>Improved Mellor-Yamada level 2 scheme, MYNN (Nakanishi and Niino 2006, JMSJ)</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>For subgrid-scale turbulence, we use improved Mellor-Yamada level 2 scheme (Nakanishi and Niino 2006, JMSJ). Other level schemes, such as level 2.5 and level 3, are also optionally available. Partial condensation scheme is also introduced (Noda et al. 2010, Atmos. Res.). Clouds are explicitly computed using one-moment or two moment bulk microphysics schemes. We generally do not use a cumulus parameterization scheme in NICAM simulations.</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>Mellor-Yamada type 2nd-order closure</t>
+  </si>
+  <si>
+    <t>Scheme Type</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>NONE</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>Not used</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>NICAM</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>non-hydrostatic model, icosahedral grid, explicit convection</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t xml:space="preserve">NICAM is a Nonhydrostatic ICosahedral Atmospheric Model (NICAM), used as a Global Cloud Resolving Model (GCRM). A subkilometer-mesh global simulation is already performed using the K computer by Miyamoto et al. (2013). NICAM is first developed by H.Tomita (JAMSTEC; now at AICS, RIKEN) and M.Satoh (AORI, The Univ. of Tokyo), and is now under development in cooperation with AORI, JAMSTEC, and RIKEN by the NICAM developers listed on http://nicam.jp/. Introduction papers of NICAM are Satoh et al. (2014, PEPS), Satoh et al.(2008, J.Comp. Physics), and Tomita and Satoh (2004, Fluid Dyn. Res.). </t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>g-level 9</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>14km lat-lon</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>14km</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloud microphysics scheme were constrained using TRMM satellite in process-oriented manner. Zonal mean zonal wind, specifically, location of midlatitude jet was used as a metric to tune the wave generation parameter in orographic gravity wave drag scheme. Surface air temperature was monitored to tune a parameter to diagnose sea ice thickness from sea ice concentration. OLR (clear &amp; cloudy), OSR (clear &amp; cloudy), precipitation and cloud fraction were often checked, though they were not a direct target of tuning this time.
+</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>Zonal mean zonal wind, surface air temperature</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>icosahedral grid</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>NICAM uses an icosahedral grid. Higher resolution grids are recursively subdivided from a coarser resolution grid. See Satoh et al. (2014) for details</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>None</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>McFarlane</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>Conventional ogographic gravity wave drag scheme by McFarlane (1987)</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>Proportional to sub-grid scale orography variance, stability and surface wind</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>Above the tropopause, extinction factor, single-scattering albedo, and asymmetry factor are considered for each band in the radiation scheme</t>
+    <phoneticPr fontId="15"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="15">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3381,6 +3474,13 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="6"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -3472,15 +3572,23 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3522,7 +3630,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3554,9 +3662,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3588,6 +3714,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3763,24 +3907,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="180.7109375" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="35.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="180.6640625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="33">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="21">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -3788,7 +3934,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" ht="21">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -3796,7 +3942,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="21">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -3804,7 +3950,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" ht="21">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -3812,7 +3958,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" ht="21">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -3820,52 +3966,52 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" ht="20.399999999999999">
       <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" ht="20.399999999999999">
       <c r="B10" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" ht="20.399999999999999">
       <c r="B11" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" ht="20.399999999999999">
       <c r="B12" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" ht="20.399999999999999">
       <c r="B13" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" ht="20.399999999999999">
       <c r="B14" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" ht="20.399999999999999">
       <c r="B15" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" ht="20.399999999999999">
       <c r="B16" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" ht="20.399999999999999">
       <c r="B17" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" ht="17.399999999999999">
       <c r="A19" s="5" t="s">
         <v>20</v>
       </c>
@@ -3873,7 +4019,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" ht="17.399999999999999">
       <c r="A20" s="5" t="s">
         <v>22</v>
       </c>
@@ -3881,7 +4027,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" ht="17.399999999999999">
       <c r="A21" s="5" t="s">
         <v>24</v>
       </c>
@@ -3889,7 +4035,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" ht="17.399999999999999">
       <c r="A22" s="5" t="s">
         <v>26</v>
       </c>
@@ -3897,39 +4043,42 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" ht="21">
       <c r="A24" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="4"/>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" ht="21">
       <c r="A25" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B25" s="4"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="15"/>
   <hyperlinks>
-    <hyperlink ref="B19" r:id="rId1"/>
-    <hyperlink ref="B20" r:id="rId2"/>
+    <hyperlink ref="B19" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B20" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD77"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:AD78"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="150.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.109375" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1">
@@ -3991,7 +4140,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="178" customHeight="1">
+    <row r="11" spans="1:3" ht="178.05" customHeight="1">
       <c r="B11" s="11"/>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
@@ -4032,7 +4181,9 @@
       </c>
     </row>
     <row r="20" spans="1:30" ht="24" customHeight="1">
-      <c r="B20" s="11"/>
+      <c r="B20" s="11" t="s">
+        <v>858</v>
+      </c>
       <c r="AA20" s="6" t="s">
         <v>857</v>
       </c>
@@ -4046,375 +4197,378 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:30" ht="24" customHeight="1">
-      <c r="A22" s="9" t="s">
+    <row r="21" spans="1:30" ht="24" customHeight="1">
+      <c r="B21" s="11" t="s">
+        <v>859</v>
+      </c>
+      <c r="AA21" s="6" t="s">
+        <v>857</v>
+      </c>
+      <c r="AB21" s="6" t="s">
+        <v>858</v>
+      </c>
+      <c r="AC21" s="6" t="s">
+        <v>859</v>
+      </c>
+      <c r="AD21" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" ht="24" customHeight="1">
+      <c r="A23" s="9" t="s">
         <v>860</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B23" s="9" t="s">
         <v>861</v>
       </c>
     </row>
-    <row r="23" spans="1:30" ht="24" customHeight="1">
-      <c r="A23" s="14" t="s">
+    <row r="24" spans="1:30" ht="24" customHeight="1">
+      <c r="A24" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B24" s="10" t="s">
         <v>862</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C24" s="10" t="s">
         <v>863</v>
       </c>
     </row>
-    <row r="24" spans="1:30" ht="24" customHeight="1">
-      <c r="B24" s="11"/>
-      <c r="AA24" s="6" t="s">
+    <row r="25" spans="1:30" ht="24" customHeight="1">
+      <c r="B25" s="11" t="s">
+        <v>865</v>
+      </c>
+      <c r="AA25" s="6" t="s">
         <v>864</v>
       </c>
-      <c r="AB24" s="6" t="s">
+      <c r="AB25" s="6" t="s">
         <v>865</v>
       </c>
-      <c r="AC24" s="6" t="s">
+      <c r="AC25" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:30" ht="24" customHeight="1">
-      <c r="A27" s="12" t="s">
+    <row r="28" spans="1:30" ht="24" customHeight="1">
+      <c r="A28" s="12" t="s">
         <v>866</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B28" s="12" t="s">
         <v>867</v>
       </c>
     </row>
-    <row r="28" spans="1:30" ht="24" customHeight="1">
-      <c r="B28" s="13" t="s">
+    <row r="29" spans="1:30" ht="24" customHeight="1">
+      <c r="B29" s="13" t="s">
         <v>868</v>
       </c>
     </row>
-    <row r="30" spans="1:30" ht="24" customHeight="1">
-      <c r="A30" s="9" t="s">
+    <row r="31" spans="1:30" ht="24" customHeight="1">
+      <c r="A31" s="9" t="s">
         <v>869</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B31" s="9" t="s">
         <v>870</v>
       </c>
     </row>
-    <row r="31" spans="1:30" ht="24" customHeight="1">
-      <c r="A31" s="14" t="s">
+    <row r="32" spans="1:30" ht="24" customHeight="1">
+      <c r="A32" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B32" s="10" t="s">
         <v>871</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C32" s="10" t="s">
         <v>872</v>
       </c>
     </row>
-    <row r="32" spans="1:30" ht="24" customHeight="1">
-      <c r="B32" s="11"/>
-      <c r="AA32" s="6" t="s">
+    <row r="33" spans="1:29" ht="24" customHeight="1">
+      <c r="B33" s="11" t="s">
+        <v>874</v>
+      </c>
+      <c r="AA33" s="6" t="s">
         <v>873</v>
       </c>
-      <c r="AB32" s="6" t="s">
+      <c r="AB33" s="6" t="s">
         <v>874</v>
       </c>
-      <c r="AC32" s="6" t="s">
+      <c r="AC33" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="24" customHeight="1">
-      <c r="A34" s="9" t="s">
+    <row r="35" spans="1:29" ht="24" customHeight="1">
+      <c r="A35" s="9" t="s">
         <v>875</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B35" s="9" t="s">
         <v>876</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="24" customHeight="1">
-      <c r="A35" s="14" t="s">
+    <row r="36" spans="1:29" ht="24" customHeight="1">
+      <c r="A36" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B36" s="10" t="s">
         <v>877</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C36" s="10" t="s">
         <v>878</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="24" customHeight="1">
-      <c r="B36" s="11"/>
-    </row>
-    <row r="38" spans="1:3" ht="24" customHeight="1">
-      <c r="A38" s="9" t="s">
+    <row r="37" spans="1:29" ht="24" customHeight="1">
+      <c r="B37" s="11"/>
+    </row>
+    <row r="39" spans="1:29" ht="24" customHeight="1">
+      <c r="A39" s="9" t="s">
         <v>879</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B39" s="9" t="s">
         <v>880</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="24" customHeight="1">
-      <c r="A39" s="14" t="s">
+    <row r="40" spans="1:29" ht="24" customHeight="1">
+      <c r="A40" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B40" s="10" t="s">
         <v>881</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C40" s="10" t="s">
         <v>882</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="24" customHeight="1">
-      <c r="B40" s="11"/>
-    </row>
-    <row r="42" spans="1:3" ht="24" customHeight="1">
-      <c r="A42" s="9" t="s">
+    <row r="41" spans="1:29" ht="24" customHeight="1">
+      <c r="B41" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:29" ht="24" customHeight="1">
+      <c r="A43" s="9" t="s">
         <v>883</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B43" s="9" t="s">
         <v>884</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="24" customHeight="1">
-      <c r="A43" s="14" t="s">
+    <row r="44" spans="1:29" ht="24" customHeight="1">
+      <c r="A44" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B44" s="10" t="s">
         <v>885</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C44" s="10" t="s">
         <v>886</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="24" customHeight="1">
-      <c r="B44" s="11"/>
-    </row>
-    <row r="47" spans="1:3" ht="24" customHeight="1">
-      <c r="A47" s="12" t="s">
+    <row r="45" spans="1:29" ht="24" customHeight="1">
+      <c r="B45" s="11"/>
+    </row>
+    <row r="48" spans="1:29" ht="24" customHeight="1">
+      <c r="A48" s="12" t="s">
         <v>887</v>
       </c>
-      <c r="B47" s="12" t="s">
+      <c r="B48" s="12" t="s">
         <v>888</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="24" customHeight="1">
-      <c r="B48" s="13" t="s">
+    <row r="49" spans="1:29" ht="24" customHeight="1">
+      <c r="B49" s="13" t="s">
         <v>889</v>
       </c>
     </row>
-    <row r="50" spans="1:29" ht="24" customHeight="1">
-      <c r="A50" s="9" t="s">
+    <row r="51" spans="1:29" ht="24" customHeight="1">
+      <c r="A51" s="9" t="s">
         <v>890</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="B51" s="9" t="s">
         <v>891</v>
       </c>
     </row>
-    <row r="51" spans="1:29" ht="24" customHeight="1">
-      <c r="A51" s="14" t="s">
+    <row r="52" spans="1:29" ht="24" customHeight="1">
+      <c r="A52" s="14" t="s">
         <v>892</v>
       </c>
-      <c r="B51" s="10" t="s">
+      <c r="B52" s="10" t="s">
         <v>893</v>
       </c>
-      <c r="C51" s="10" t="s">
+      <c r="C52" s="10" t="s">
         <v>894</v>
       </c>
     </row>
-    <row r="52" spans="1:29" ht="24" customHeight="1">
-      <c r="B52" s="11"/>
-    </row>
-    <row r="54" spans="1:29" ht="24" customHeight="1">
-      <c r="A54" s="9" t="s">
+    <row r="53" spans="1:29" ht="24" customHeight="1">
+      <c r="B53" s="11"/>
+    </row>
+    <row r="55" spans="1:29" ht="24" customHeight="1">
+      <c r="A55" s="9" t="s">
         <v>895</v>
       </c>
-      <c r="B54" s="9" t="s">
+      <c r="B55" s="9" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="55" spans="1:29" ht="24" customHeight="1">
-      <c r="A55" s="14" t="s">
+    <row r="56" spans="1:29" ht="24" customHeight="1">
+      <c r="A56" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="B55" s="10" t="s">
+      <c r="B56" s="10" t="s">
         <v>896</v>
       </c>
-      <c r="C55" s="10" t="s">
+      <c r="C56" s="10" t="s">
         <v>897</v>
       </c>
     </row>
-    <row r="56" spans="1:29" ht="24" customHeight="1">
-      <c r="B56" s="11"/>
-      <c r="AA56" s="6" t="s">
+    <row r="57" spans="1:29" ht="24" customHeight="1">
+      <c r="B57" s="11"/>
+      <c r="AA57" s="6" t="s">
         <v>898</v>
       </c>
-      <c r="AB56" s="6" t="s">
+      <c r="AB57" s="6" t="s">
         <v>899</v>
       </c>
-      <c r="AC56" s="6" t="s">
+      <c r="AC57" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="58" spans="1:29" ht="24" customHeight="1">
-      <c r="A58" s="9" t="s">
+    <row r="59" spans="1:29" ht="24" customHeight="1">
+      <c r="A59" s="9" t="s">
         <v>900</v>
       </c>
-      <c r="B58" s="9" t="s">
+      <c r="B59" s="9" t="s">
         <v>901</v>
       </c>
     </row>
-    <row r="59" spans="1:29" ht="24" customHeight="1">
-      <c r="A59" s="14" t="s">
+    <row r="60" spans="1:29" ht="24" customHeight="1">
+      <c r="A60" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="B59" s="10" t="s">
+      <c r="B60" s="10" t="s">
         <v>902</v>
       </c>
-      <c r="C59" s="10" t="s">
+      <c r="C60" s="10" t="s">
         <v>903</v>
       </c>
     </row>
-    <row r="60" spans="1:29" ht="24" customHeight="1">
-      <c r="B60" s="11"/>
-    </row>
-    <row r="62" spans="1:29" ht="24" customHeight="1">
-      <c r="A62" s="9" t="s">
+    <row r="61" spans="1:29" ht="24" customHeight="1">
+      <c r="B61" s="11"/>
+    </row>
+    <row r="63" spans="1:29" ht="24" customHeight="1">
+      <c r="A63" s="9" t="s">
         <v>904</v>
       </c>
-      <c r="B62" s="9" t="s">
+      <c r="B63" s="9" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="63" spans="1:29" ht="24" customHeight="1">
-      <c r="A63" s="14" t="s">
+    <row r="64" spans="1:29" ht="24" customHeight="1">
+      <c r="A64" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="B63" s="10" t="s">
+      <c r="B64" s="10" t="s">
         <v>906</v>
       </c>
-      <c r="C63" s="10" t="s">
+      <c r="C64" s="10" t="s">
         <v>907</v>
       </c>
     </row>
-    <row r="64" spans="1:29" ht="24" customHeight="1">
-      <c r="B64" s="11"/>
-    </row>
-    <row r="67" spans="1:29" ht="24" customHeight="1">
-      <c r="A67" s="12" t="s">
+    <row r="65" spans="1:29" ht="24" customHeight="1">
+      <c r="B65" s="11"/>
+    </row>
+    <row r="68" spans="1:29" ht="24" customHeight="1">
+      <c r="A68" s="12" t="s">
         <v>908</v>
       </c>
-      <c r="B67" s="12" t="s">
+      <c r="B68" s="12" t="s">
         <v>909</v>
       </c>
     </row>
-    <row r="68" spans="1:29" ht="24" customHeight="1">
-      <c r="B68" s="13" t="s">
+    <row r="69" spans="1:29" ht="24" customHeight="1">
+      <c r="B69" s="13" t="s">
         <v>910</v>
       </c>
     </row>
-    <row r="70" spans="1:29" ht="24" customHeight="1">
-      <c r="A70" s="9" t="s">
+    <row r="71" spans="1:29" ht="24" customHeight="1">
+      <c r="A71" s="9" t="s">
         <v>911</v>
       </c>
-      <c r="B70" s="9" t="s">
+      <c r="B71" s="9" t="s">
         <v>912</v>
       </c>
     </row>
-    <row r="71" spans="1:29" ht="24" customHeight="1">
-      <c r="A71" s="14" t="s">
+    <row r="72" spans="1:29" ht="24" customHeight="1">
+      <c r="A72" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="B71" s="10" t="s">
+      <c r="B72" s="10" t="s">
         <v>913</v>
       </c>
-      <c r="C71" s="10" t="s">
+      <c r="C72" s="10" t="s">
         <v>914</v>
       </c>
     </row>
-    <row r="72" spans="1:29" ht="24" customHeight="1">
-      <c r="B72" s="11"/>
-      <c r="AA72" s="6" t="s">
+    <row r="73" spans="1:29" ht="24" customHeight="1">
+      <c r="B73" s="11"/>
+      <c r="AA73" s="6" t="s">
         <v>915</v>
       </c>
-      <c r="AB72" s="6" t="s">
+      <c r="AB73" s="6" t="s">
         <v>916</v>
       </c>
-      <c r="AC72" s="6" t="s">
+      <c r="AC73" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="74" spans="1:29" ht="24" customHeight="1">
-      <c r="A74" s="9" t="s">
+    <row r="75" spans="1:29" ht="24" customHeight="1">
+      <c r="A75" s="9" t="s">
         <v>917</v>
       </c>
-      <c r="B74" s="9" t="s">
+      <c r="B75" s="9" t="s">
         <v>918</v>
       </c>
     </row>
-    <row r="75" spans="1:29" ht="24" customHeight="1">
-      <c r="A75" s="14" t="s">
+    <row r="76" spans="1:29" ht="24" customHeight="1">
+      <c r="A76" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="B75" s="10" t="s">
+      <c r="B76" s="10" t="s">
         <v>919</v>
       </c>
-      <c r="C75" s="10" t="s">
+      <c r="C76" s="10" t="s">
         <v>920</v>
       </c>
     </row>
-    <row r="76" spans="1:29" ht="24" customHeight="1">
-      <c r="B76" s="10" t="s">
+    <row r="77" spans="1:29" ht="24" customHeight="1">
+      <c r="B77" s="10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="77" spans="1:29" ht="24" customHeight="1">
-      <c r="B77" s="11"/>
-      <c r="AA77" s="6" t="s">
+    <row r="78" spans="1:29" ht="24" customHeight="1">
+      <c r="B78" s="11"/>
+      <c r="AA78" s="6" t="s">
         <v>921</v>
       </c>
-      <c r="AB77" s="6" t="s">
+      <c r="AB78" s="6" t="s">
         <v>798</v>
       </c>
-      <c r="AC77" s="6" t="s">
+      <c r="AC78" s="6" t="s">
         <v>66</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20">
+  <phoneticPr fontId="15"/>
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20:B21" xr:uid="{00000000-0002-0000-0900-000000000000}">
       <formula1>AA20:AD20</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24">
-      <formula1>AA24:AC24</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B25 B78 B73 B57 B33" xr:uid="{00000000-0002-0000-0900-000001000000}">
+      <formula1>AA25:AC25</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B32">
-      <formula1>AA32:AC32</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B36">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B37 B45 B41" xr:uid="{00000000-0002-0000-0900-000003000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B40">
-      <formula1>0</formula1>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B53" xr:uid="{00000000-0002-0000-0900-000006000000}">
+      <formula1>-1000000</formula1>
+      <formula2>1000000</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B44">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B52">
-      <formula1>-1000000.0</formula1>
-      <formula2>1000000.0</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B56">
-      <formula1>AA56:AC56</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B60">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B61 B65" xr:uid="{00000000-0002-0000-0900-000008000000}">
       <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B64">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B72">
-      <formula1>AA72:AC72</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B77">
-      <formula1>AA77:AC77</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4422,17 +4576,19 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD76"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:AF76"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="D77" sqref="D77"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="150.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.109375" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="24" customHeight="1">
@@ -4468,7 +4624,9 @@
       </c>
     </row>
     <row r="6" spans="1:29" ht="24" customHeight="1">
-      <c r="B6" s="11"/>
+      <c r="B6" s="11" t="s">
+        <v>1101</v>
+      </c>
     </row>
     <row r="8" spans="1:29" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
@@ -4494,8 +4652,10 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="178" customHeight="1">
-      <c r="B11" s="11"/>
+    <row r="11" spans="1:29" ht="178.05" customHeight="1">
+      <c r="B11" s="11" t="s">
+        <v>1102</v>
+      </c>
     </row>
     <row r="13" spans="1:29" ht="24" customHeight="1">
       <c r="A13" s="9" t="s">
@@ -4517,7 +4677,9 @@
       </c>
     </row>
     <row r="15" spans="1:29" ht="24" customHeight="1">
-      <c r="B15" s="11"/>
+      <c r="B15" s="11" t="s">
+        <v>936</v>
+      </c>
       <c r="AA15" s="6" t="s">
         <v>935</v>
       </c>
@@ -4548,7 +4710,9 @@
       </c>
     </row>
     <row r="19" spans="1:30" ht="24" customHeight="1">
-      <c r="B19" s="11"/>
+      <c r="B19" s="11" t="s">
+        <v>941</v>
+      </c>
       <c r="AA19" s="6" t="s">
         <v>941</v>
       </c>
@@ -4584,7 +4748,9 @@
       </c>
     </row>
     <row r="24" spans="1:30" ht="24" customHeight="1">
-      <c r="B24" s="11"/>
+      <c r="B24" s="11" t="s">
+        <v>947</v>
+      </c>
       <c r="AA24" s="6" t="s">
         <v>947</v>
       </c>
@@ -4631,7 +4797,9 @@
       </c>
     </row>
     <row r="32" spans="1:30" ht="24" customHeight="1">
-      <c r="B32" s="11"/>
+      <c r="B32" s="11" t="s">
+        <v>1101</v>
+      </c>
     </row>
     <row r="34" spans="1:32" ht="24" customHeight="1">
       <c r="A34" s="9" t="s">
@@ -4658,7 +4826,9 @@
       </c>
     </row>
     <row r="37" spans="1:32" ht="24" customHeight="1">
-      <c r="B37" s="11"/>
+      <c r="B37" s="11" t="s">
+        <v>964</v>
+      </c>
       <c r="AA37" s="6" t="s">
         <v>960</v>
       </c>
@@ -4703,7 +4873,12 @@
       </c>
     </row>
     <row r="42" spans="1:32" ht="24" customHeight="1">
-      <c r="B42" s="11"/>
+      <c r="B42" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>1103</v>
+      </c>
       <c r="AA42" s="6" t="s">
         <v>969</v>
       </c>
@@ -4734,7 +4909,9 @@
       </c>
     </row>
     <row r="46" spans="1:32" ht="24" customHeight="1">
-      <c r="B46" s="11"/>
+      <c r="B46" s="11" t="s">
+        <v>975</v>
+      </c>
       <c r="AA46" s="6" t="s">
         <v>975</v>
       </c>
@@ -4768,7 +4945,9 @@
       </c>
     </row>
     <row r="50" spans="1:32" ht="24" customHeight="1">
-      <c r="B50" s="11"/>
+      <c r="B50" s="11" t="s">
+        <v>984</v>
+      </c>
       <c r="AA50" s="6" t="s">
         <v>982</v>
       </c>
@@ -4821,7 +5000,9 @@
       </c>
     </row>
     <row r="58" spans="1:32" ht="24" customHeight="1">
-      <c r="B58" s="11"/>
+      <c r="B58" s="11" t="s">
+        <v>1100</v>
+      </c>
     </row>
     <row r="60" spans="1:32" ht="24" customHeight="1">
       <c r="A60" s="9" t="s">
@@ -4848,7 +5029,12 @@
       </c>
     </row>
     <row r="63" spans="1:32" ht="24" customHeight="1">
-      <c r="B63" s="11"/>
+      <c r="B63" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>1089</v>
+      </c>
       <c r="AA63" s="6" t="s">
         <v>994</v>
       </c>
@@ -4888,6 +5074,9 @@
     </row>
     <row r="68" spans="1:32" ht="24" customHeight="1">
       <c r="B68" s="11"/>
+      <c r="D68" s="6" t="s">
+        <v>1089</v>
+      </c>
       <c r="AA68" s="6" t="s">
         <v>1000</v>
       </c>
@@ -4916,6 +5105,9 @@
     </row>
     <row r="72" spans="1:32" ht="24" customHeight="1">
       <c r="B72" s="11"/>
+      <c r="D72" s="6" t="s">
+        <v>1089</v>
+      </c>
       <c r="AA72" s="6" t="s">
         <v>975</v>
       </c>
@@ -4947,6 +5139,9 @@
     </row>
     <row r="76" spans="1:32" ht="24" customHeight="1">
       <c r="B76" s="11"/>
+      <c r="D76" s="6" t="s">
+        <v>1089</v>
+      </c>
       <c r="AA76" s="6" t="s">
         <v>982</v>
       </c>
@@ -4967,39 +5162,19 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="11">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+  <phoneticPr fontId="15"/>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15 B72 B42 B19" xr:uid="{00000000-0002-0000-0A00-000000000000}">
       <formula1>AA15:AC15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19">
-      <formula1>AA19:AC19</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24 B63 B46" xr:uid="{00000000-0002-0000-0A00-000002000000}">
       <formula1>AA24:AD24</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B37">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B37 B76 B50" xr:uid="{00000000-0002-0000-0A00-000003000000}">
       <formula1>AA37:AF37</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B42">
-      <formula1>AA42:AC42</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B46">
-      <formula1>AA46:AD46</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B50">
-      <formula1>AA50:AF50</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B63">
-      <formula1>AA63:AD63</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B68">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B68" xr:uid="{00000000-0002-0000-0A00-000008000000}">
       <formula1>AA68:AB68</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B72">
-      <formula1>AA72:AC72</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B76">
-      <formula1>AA76:AF76</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5007,17 +5182,19 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD77"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1:AD77"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="150.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.109375" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1">
@@ -5079,7 +5256,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="178" customHeight="1">
+    <row r="11" spans="1:3" ht="178.05" customHeight="1">
       <c r="B11" s="11"/>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
@@ -5120,7 +5297,9 @@
       </c>
     </row>
     <row r="20" spans="1:30" ht="24" customHeight="1">
-      <c r="B20" s="11"/>
+      <c r="B20" s="11" t="s">
+        <v>1024</v>
+      </c>
       <c r="AA20" s="6" t="s">
         <v>1024</v>
       </c>
@@ -5167,7 +5346,9 @@
       </c>
     </row>
     <row r="28" spans="1:30" ht="24" customHeight="1">
-      <c r="B28" s="11"/>
+      <c r="B28" s="11" t="s">
+        <v>1034</v>
+      </c>
       <c r="AA28" s="6" t="s">
         <v>1033</v>
       </c>
@@ -5252,7 +5433,9 @@
       </c>
     </row>
     <row r="44" spans="1:28" ht="24" customHeight="1">
-      <c r="B44" s="11"/>
+      <c r="B44" s="11" t="s">
+        <v>1033</v>
+      </c>
       <c r="AA44" s="6" t="s">
         <v>1033</v>
       </c>
@@ -5368,7 +5551,9 @@
       </c>
     </row>
     <row r="64" spans="1:29" ht="24" customHeight="1">
-      <c r="B64" s="11"/>
+      <c r="B64" s="11" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="67" spans="1:29" ht="24" customHeight="1">
       <c r="A67" s="12" t="s">
@@ -5407,8 +5592,10 @@
         <v>58</v>
       </c>
     </row>
-    <row r="73" spans="1:29" ht="178" customHeight="1">
-      <c r="B73" s="11"/>
+    <row r="73" spans="1:29" ht="178.05" customHeight="1">
+      <c r="B73" s="11" t="s">
+        <v>1104</v>
+      </c>
     </row>
     <row r="75" spans="1:29" ht="24" customHeight="1">
       <c r="A75" s="9" t="s">
@@ -5430,7 +5617,9 @@
       </c>
     </row>
     <row r="77" spans="1:29" ht="24" customHeight="1">
-      <c r="B77" s="11"/>
+      <c r="B77" s="11" t="s">
+        <v>1082</v>
+      </c>
       <c r="AA77" s="6" t="s">
         <v>1081</v>
       </c>
@@ -5442,51 +5631,47 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="8">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20">
+  <phoneticPr fontId="15"/>
+  <dataValidations count="6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20" xr:uid="{00000000-0002-0000-0B00-000000000000}">
       <formula1>AA20:AD20</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B28">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B28 B44" xr:uid="{00000000-0002-0000-0B00-000001000000}">
       <formula1>AA28:AB28</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B32">
-      <formula1>-1000000.0</formula1>
-      <formula2>1000000.0</formula2>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B32" xr:uid="{00000000-0002-0000-0B00-000002000000}">
+      <formula1>-1000000</formula1>
+      <formula2>1000000</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B44">
-      <formula1>AA44:AB44</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B48">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B48" xr:uid="{00000000-0002-0000-0B00-000004000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B56">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B56 B77" xr:uid="{00000000-0002-0000-0B00-000005000000}">
       <formula1>AA56:AC56</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B64">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B64" xr:uid="{00000000-0002-0000-0B00-000006000000}">
       <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B77">
-      <formula1>AA77:AC77</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="80.7109375" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="80.6640625" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" customWidth="1"/>
+    <col min="3" max="16384" width="9.109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="30">
       <c r="A1" s="7" t="s">
         <v>30</v>
       </c>
@@ -5497,7 +5682,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="17.399999999999999">
       <c r="A5" s="9" t="s">
         <v>32</v>
       </c>
@@ -5513,7 +5698,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" ht="15.6">
       <c r="A8" s="10" t="s">
         <v>35</v>
       </c>
@@ -5521,11 +5706,11 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" ht="17.399999999999999">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" ht="17.399999999999999">
       <c r="A12" s="9" t="s">
         <v>37</v>
       </c>
@@ -5541,7 +5726,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" ht="15.6">
       <c r="A16" s="10" t="s">
         <v>35</v>
       </c>
@@ -5549,39 +5734,42 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" ht="17.399999999999999">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="15"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Author,Contributor,Principal Investigator,Point of Contact,Sponsor"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Top Level,Key Properties,Grid,Dynamical Core,Radiation,Turbulence Convection,Microphysics Precipitation,Cloud Scheme,Observation Simulation,Gravity Waves,Natural Forcing"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1"/>
-    <hyperlink ref="A13" r:id="rId2"/>
+    <hyperlink ref="A6" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="A13" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD106"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AG106"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="150.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.109375" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1">
@@ -5617,7 +5805,9 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1">
-      <c r="B6" s="11"/>
+      <c r="B6" s="11" t="s">
+        <v>1090</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
@@ -5644,7 +5834,9 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="24" customHeight="1">
-      <c r="B11" s="11"/>
+      <c r="B11" s="11" t="s">
+        <v>1091</v>
+      </c>
     </row>
     <row r="13" spans="1:3" ht="24" customHeight="1">
       <c r="A13" s="9" t="s">
@@ -5670,8 +5862,10 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="178" customHeight="1">
-      <c r="B16" s="11"/>
+    <row r="16" spans="1:3" ht="178.05" customHeight="1">
+      <c r="B16" s="11" t="s">
+        <v>1092</v>
+      </c>
     </row>
     <row r="18" spans="1:33" ht="24" customHeight="1">
       <c r="A18" s="9" t="s">
@@ -5693,7 +5887,9 @@
       </c>
     </row>
     <row r="20" spans="1:33" ht="24" customHeight="1">
-      <c r="B20" s="11"/>
+      <c r="B20" s="11" t="s">
+        <v>64</v>
+      </c>
       <c r="AA20" s="6" t="s">
         <v>64</v>
       </c>
@@ -5729,7 +5925,9 @@
       </c>
     </row>
     <row r="25" spans="1:33" ht="24" customHeight="1">
-      <c r="B25" s="11"/>
+      <c r="B25" s="11" t="s">
+        <v>72</v>
+      </c>
       <c r="AA25" s="6" t="s">
         <v>71</v>
       </c>
@@ -5785,7 +5983,9 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="24" customHeight="1">
-      <c r="B33" s="11"/>
+      <c r="B33" s="11" t="s">
+        <v>1093</v>
+      </c>
     </row>
     <row r="35" spans="1:3" ht="24" customHeight="1">
       <c r="A35" s="9" t="s">
@@ -5807,7 +6007,9 @@
       </c>
     </row>
     <row r="37" spans="1:3" ht="24" customHeight="1">
-      <c r="B37" s="11"/>
+      <c r="B37" s="11" t="s">
+        <v>1094</v>
+      </c>
     </row>
     <row r="39" spans="1:3" ht="24" customHeight="1">
       <c r="A39" s="9" t="s">
@@ -5829,7 +6031,9 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="24" customHeight="1">
-      <c r="B41" s="11"/>
+      <c r="B41" s="11" t="s">
+        <v>1095</v>
+      </c>
     </row>
     <row r="43" spans="1:3" ht="24" customHeight="1">
       <c r="A43" s="9" t="s">
@@ -5851,7 +6055,9 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="24" customHeight="1">
-      <c r="B45" s="11"/>
+      <c r="B45" s="11">
+        <v>38</v>
+      </c>
     </row>
     <row r="47" spans="1:3" ht="24" customHeight="1">
       <c r="A47" s="9" t="s">
@@ -5873,7 +6079,9 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="24" customHeight="1">
-      <c r="B49" s="11"/>
+      <c r="B49" s="11" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="52" spans="1:3" ht="24" customHeight="1">
       <c r="A52" s="12" t="s">
@@ -5908,7 +6116,9 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="24" customHeight="1">
-      <c r="B57" s="11"/>
+      <c r="B57" s="11">
+        <v>60</v>
+      </c>
     </row>
     <row r="59" spans="1:3" ht="24" customHeight="1">
       <c r="A59" s="9" t="s">
@@ -5930,7 +6140,9 @@
       </c>
     </row>
     <row r="61" spans="1:3" ht="24" customHeight="1">
-      <c r="B61" s="11"/>
+      <c r="B61" s="11">
+        <v>600</v>
+      </c>
     </row>
     <row r="63" spans="1:3" ht="24" customHeight="1">
       <c r="A63" s="9" t="s">
@@ -5952,7 +6164,9 @@
       </c>
     </row>
     <row r="65" spans="1:31" ht="24" customHeight="1">
-      <c r="B65" s="11"/>
+      <c r="B65" s="11">
+        <v>600</v>
+      </c>
     </row>
     <row r="68" spans="1:31" ht="24" customHeight="1">
       <c r="A68" s="12" t="s">
@@ -5987,7 +6201,9 @@
       </c>
     </row>
     <row r="73" spans="1:31" ht="24" customHeight="1">
-      <c r="B73" s="11"/>
+      <c r="B73" s="11" t="s">
+        <v>124</v>
+      </c>
       <c r="AA73" s="6" t="s">
         <v>124</v>
       </c>
@@ -6099,8 +6315,10 @@
         <v>58</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="178" customHeight="1">
-      <c r="B91" s="11"/>
+    <row r="91" spans="1:3" ht="178.05" customHeight="1">
+      <c r="B91" s="11" t="s">
+        <v>1096</v>
+      </c>
     </row>
     <row r="93" spans="1:3" ht="24" customHeight="1">
       <c r="A93" s="9" t="s">
@@ -6127,7 +6345,9 @@
       </c>
     </row>
     <row r="96" spans="1:3" ht="24" customHeight="1">
-      <c r="B96" s="11"/>
+      <c r="B96" s="11" t="s">
+        <v>1097</v>
+      </c>
     </row>
     <row r="98" spans="1:3" ht="24" customHeight="1">
       <c r="A98" s="9" t="s">
@@ -6154,7 +6374,9 @@
       </c>
     </row>
     <row r="101" spans="1:3" ht="24" customHeight="1">
-      <c r="B101" s="11"/>
+      <c r="B101" s="11" t="s">
+        <v>1089</v>
+      </c>
     </row>
     <row r="103" spans="1:3" ht="24" customHeight="1">
       <c r="A103" s="9" t="s">
@@ -6181,35 +6403,26 @@
       </c>
     </row>
     <row r="106" spans="1:3" ht="24" customHeight="1">
-      <c r="B106" s="11"/>
+      <c r="B106" s="11" t="s">
+        <v>1089</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="9">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20">
+  <phoneticPr fontId="15"/>
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20 B73" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>AA20:AC20</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B25" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>AA25:AG25</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B45">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B45 B65 B61 B57" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B49">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B49" xr:uid="{00000000-0002-0000-0200-000003000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B57">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B61">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B65">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B73">
-      <formula1>AA73:AC73</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B78">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B78" xr:uid="{00000000-0002-0000-0200-000008000000}">
       <formula1>AA78:AE78</formula1>
     </dataValidation>
   </dataValidations>
@@ -6218,17 +6431,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:AF44"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="150.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.109375" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1">
@@ -6264,7 +6479,9 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1">
-      <c r="B6" s="11"/>
+      <c r="B6" s="11" t="s">
+        <v>1098</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
@@ -6290,8 +6507,10 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="178" customHeight="1">
-      <c r="B11" s="11"/>
+    <row r="11" spans="1:3" ht="178.05" customHeight="1">
+      <c r="B11" s="11" t="s">
+        <v>1099</v>
+      </c>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
       <c r="A14" s="12" t="s">
@@ -6535,23 +6754,18 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19">
+  <phoneticPr fontId="15"/>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>AA19:AC19</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23 B31 B27" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>AA23:AD23</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B27">
-      <formula1>AA27:AD27</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B31">
-      <formula1>AA31:AD31</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B35" xr:uid="{00000000-0002-0000-0300-000004000000}">
       <formula1>AA35:AE35</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B44">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B44" xr:uid="{00000000-0002-0000-0300-000005000000}">
       <formula1>AA44:AF44</formula1>
     </dataValidation>
   </dataValidations>
@@ -6560,17 +6774,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD104"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:AM104"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="150.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.109375" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="24" customHeight="1">
@@ -6632,7 +6846,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:36" ht="178" customHeight="1">
+    <row r="11" spans="1:36" ht="178.05" customHeight="1">
       <c r="B11" s="11"/>
     </row>
     <row r="13" spans="1:36" ht="24" customHeight="1">
@@ -7343,47 +7557,30 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="14">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+  <phoneticPr fontId="15"/>
+  <dataValidations count="8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>AA15:AJ15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20 B69" xr:uid="{00000000-0002-0000-0400-000001000000}">
       <formula1>AA20:AM20</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B28">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B28 B78 B74 B56 B44" xr:uid="{00000000-0002-0000-0400-000002000000}">
       <formula1>AA28:AC28</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B44">
-      <formula1>AA44:AC44</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B56">
-      <formula1>AA56:AC56</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B64">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B64 B91" xr:uid="{00000000-0002-0000-0400-000005000000}">
       <formula1>AA64:AF64</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B69">
-      <formula1>AA69:AM69</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B74">
-      <formula1>AA74:AC74</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B78">
-      <formula1>AA78:AC78</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B86">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B86" xr:uid="{00000000-0002-0000-0400-000009000000}">
       <formula1>AA86:AD86</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B91">
-      <formula1>AA91:AF91</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B95">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B95" xr:uid="{00000000-0002-0000-0400-00000B000000}">
       <formula1>AA95:AE95</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B100">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B100" xr:uid="{00000000-0002-0000-0400-00000C000000}">
       <formula1>AA100:AG100</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B104">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B104" xr:uid="{00000000-0002-0000-0400-00000D000000}">
       <formula1>AA104:AB104</formula1>
     </dataValidation>
   </dataValidations>
@@ -7392,17 +7589,17 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD206"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:AX206"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="150.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.109375" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="24" customHeight="1">
@@ -7464,7 +7661,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:40" ht="178" customHeight="1">
+    <row r="11" spans="1:40" ht="178.05" customHeight="1">
       <c r="B11" s="11"/>
     </row>
     <row r="13" spans="1:40" ht="24" customHeight="1">
@@ -9093,93 +9290,40 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="29">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16">
+  <phoneticPr fontId="15"/>
+  <dataValidations count="11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>AA16:AN16</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B28">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B28 B192 B123 B97" xr:uid="{00000000-0002-0000-0500-000001000000}">
       <formula1>AA28:AD28</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B33">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B33 B206 B170 B128 B111 B75" xr:uid="{00000000-0002-0000-0500-000002000000}">
       <formula1>AA33:AF33</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B37">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B37 B132" xr:uid="{00000000-0002-0000-0500-000003000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B42">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B42 B184 B137 B89" xr:uid="{00000000-0002-0000-0500-000004000000}">
       <formula1>AA42:AC42</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B51">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B51 B146" xr:uid="{00000000-0002-0000-0500-000005000000}">
       <formula1>AA51:AK51</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B56">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B56 B151" xr:uid="{00000000-0002-0000-0500-000006000000}">
       <formula1>AA56:AR56</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B61">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B61 B156" xr:uid="{00000000-0002-0000-0500-000007000000}">
       <formula1>AA61:AX61</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B70">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B70 B165" xr:uid="{00000000-0002-0000-0500-000008000000}">
       <formula1>AA70:AH70</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B75">
-      <formula1>AA75:AF75</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B84">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B84 B179" xr:uid="{00000000-0002-0000-0500-00000A000000}">
       <formula1>AA84:AE84</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B89">
-      <formula1>AA89:AC89</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B97">
-      <formula1>AA97:AD97</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B106">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B106 B201" xr:uid="{00000000-0002-0000-0500-00000D000000}">
       <formula1>AA106:AG106</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B111">
-      <formula1>AA111:AF111</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B123">
-      <formula1>AA123:AD123</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B128">
-      <formula1>AA128:AF128</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B132">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B137">
-      <formula1>AA137:AC137</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B146">
-      <formula1>AA146:AK146</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B151">
-      <formula1>AA151:AR151</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B156">
-      <formula1>AA156:AX156</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B165">
-      <formula1>AA165:AH165</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B170">
-      <formula1>AA170:AF170</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B179">
-      <formula1>AA179:AE179</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B184">
-      <formula1>AA184:AC184</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B192">
-      <formula1>AA192:AD192</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B201">
-      <formula1>AA201:AG201</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B206">
-      <formula1>AA206:AF206</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9187,17 +9331,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD87"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:AK87"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="150.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.109375" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1">
@@ -9233,7 +9379,9 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1">
-      <c r="B6" s="11"/>
+      <c r="B6" s="11" t="s">
+        <v>1084</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
@@ -9259,8 +9407,10 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="178" customHeight="1">
-      <c r="B11" s="11"/>
+    <row r="11" spans="1:3" ht="178.05" customHeight="1">
+      <c r="B11" s="11" t="s">
+        <v>1085</v>
+      </c>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
       <c r="A14" s="12" t="s">
@@ -9295,7 +9445,12 @@
       </c>
     </row>
     <row r="19" spans="1:37" ht="24" customHeight="1">
-      <c r="B19" s="11"/>
+      <c r="B19" s="11" t="s">
+        <v>627</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>1083</v>
+      </c>
       <c r="AA19" s="6" t="s">
         <v>627</v>
       </c>
@@ -9314,7 +9469,7 @@
         <v>630</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>170</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="22" spans="1:37" ht="24" customHeight="1">
@@ -9334,7 +9489,12 @@
       </c>
     </row>
     <row r="24" spans="1:37" ht="24" customHeight="1">
-      <c r="B24" s="11"/>
+      <c r="B24" s="11" t="s">
+        <v>634</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>1086</v>
+      </c>
       <c r="AA24" s="6" t="s">
         <v>633</v>
       </c>
@@ -9389,7 +9549,9 @@
       </c>
     </row>
     <row r="28" spans="1:37" ht="24" customHeight="1">
-      <c r="B28" s="11"/>
+      <c r="B28" s="11">
+        <v>2</v>
+      </c>
     </row>
     <row r="30" spans="1:37" ht="24" customHeight="1">
       <c r="A30" s="9" t="s">
@@ -9411,7 +9573,9 @@
       </c>
     </row>
     <row r="32" spans="1:37" ht="24" customHeight="1">
-      <c r="B32" s="11"/>
+      <c r="B32" s="11" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="1:30" ht="24" customHeight="1">
       <c r="A35" s="12" t="s">
@@ -9446,7 +9610,9 @@
       </c>
     </row>
     <row r="40" spans="1:30" ht="24" customHeight="1">
-      <c r="B40" s="11"/>
+      <c r="B40" s="11" t="s">
+        <v>1088</v>
+      </c>
     </row>
     <row r="42" spans="1:30" ht="24" customHeight="1">
       <c r="A42" s="9" t="s">
@@ -9473,7 +9639,12 @@
       </c>
     </row>
     <row r="45" spans="1:30" ht="24" customHeight="1">
-      <c r="B45" s="11"/>
+      <c r="B45" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>1089</v>
+      </c>
       <c r="AA45" s="6" t="s">
         <v>660</v>
       </c>
@@ -9512,7 +9683,12 @@
       </c>
     </row>
     <row r="50" spans="1:36" ht="24" customHeight="1">
-      <c r="B50" s="11"/>
+      <c r="B50" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>1089</v>
+      </c>
       <c r="AA50" s="6" t="s">
         <v>666</v>
       </c>
@@ -9558,6 +9734,9 @@
     </row>
     <row r="55" spans="1:36" ht="24" customHeight="1">
       <c r="B55" s="11"/>
+      <c r="D55" s="6" t="s">
+        <v>1089</v>
+      </c>
       <c r="AA55" s="6" t="s">
         <v>674</v>
       </c>
@@ -9614,7 +9793,9 @@
       </c>
     </row>
     <row r="60" spans="1:36" ht="24" customHeight="1">
-      <c r="B60" s="11"/>
+      <c r="B60" s="11" t="s">
+        <v>688</v>
+      </c>
       <c r="AA60" s="6" t="s">
         <v>687</v>
       </c>
@@ -9661,7 +9842,9 @@
       </c>
     </row>
     <row r="68" spans="1:30" ht="24" customHeight="1">
-      <c r="B68" s="11"/>
+      <c r="B68" s="11" t="s">
+        <v>1088</v>
+      </c>
     </row>
     <row r="70" spans="1:30" ht="24" customHeight="1">
       <c r="A70" s="9" t="s">
@@ -9688,7 +9871,12 @@
       </c>
     </row>
     <row r="73" spans="1:30" ht="24" customHeight="1">
-      <c r="B73" s="11"/>
+      <c r="B73" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>1089</v>
+      </c>
       <c r="AA73" s="6" t="s">
         <v>660</v>
       </c>
@@ -9719,7 +9907,12 @@
       </c>
     </row>
     <row r="77" spans="1:30" ht="24" customHeight="1">
-      <c r="B77" s="11"/>
+      <c r="B77" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>1089</v>
+      </c>
       <c r="AA77" s="6" t="s">
         <v>703</v>
       </c>
@@ -9758,7 +9951,12 @@
       </c>
     </row>
     <row r="82" spans="1:32" ht="24" customHeight="1">
-      <c r="B82" s="11"/>
+      <c r="B82" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>1089</v>
+      </c>
       <c r="AA82" s="6" t="s">
         <v>675</v>
       </c>
@@ -9803,7 +10001,9 @@
       </c>
     </row>
     <row r="87" spans="1:32" ht="24" customHeight="1">
-      <c r="B87" s="11"/>
+      <c r="B87" s="11" t="s">
+        <v>688</v>
+      </c>
       <c r="AA87" s="6" t="s">
         <v>687</v>
       </c>
@@ -9818,42 +10018,28 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19">
+  <phoneticPr fontId="15"/>
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19 B87 B77 B60 B45" xr:uid="{00000000-0002-0000-0600-000000000000}">
       <formula1>AA19:AD19</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24" xr:uid="{00000000-0002-0000-0600-000001000000}">
       <formula1>AA24:AK24</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B28">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B28" xr:uid="{00000000-0002-0000-0600-000002000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B32" xr:uid="{00000000-0002-0000-0600-000003000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B45">
-      <formula1>AA45:AD45</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B50">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B50 B82" xr:uid="{00000000-0002-0000-0600-000005000000}">
       <formula1>AA50:AF50</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B55">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B55" xr:uid="{00000000-0002-0000-0600-000006000000}">
       <formula1>AA55:AJ55</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B60">
-      <formula1>AA60:AD60</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B73">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B73" xr:uid="{00000000-0002-0000-0600-000008000000}">
       <formula1>AA73:AC73</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B77">
-      <formula1>AA77:AD77</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82">
-      <formula1>AA82:AF82</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B87">
-      <formula1>AA87:AD87</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9861,17 +10047,17 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:AI37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="150.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.109375" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1">
@@ -9933,7 +10119,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="178" customHeight="1">
+    <row r="11" spans="1:3" ht="178.05" customHeight="1">
       <c r="B11" s="11"/>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
@@ -10103,11 +10289,12 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="15"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24" xr:uid="{00000000-0002-0000-0700-000000000000}">
       <formula1>AA24:AE24</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B37">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B37" xr:uid="{00000000-0002-0000-0700-000001000000}">
       <formula1>AA37:AI37</formula1>
     </dataValidation>
   </dataValidations>
@@ -10116,17 +10303,17 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD89"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:AH89"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="150.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.109375" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="24" customHeight="1">
@@ -10188,7 +10375,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="178" customHeight="1">
+    <row r="11" spans="1:29" ht="178.05" customHeight="1">
       <c r="B11" s="11"/>
     </row>
     <row r="13" spans="1:29" ht="24" customHeight="1">
@@ -10699,39 +10886,28 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="11">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16">
+  <phoneticPr fontId="15"/>
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16 B89 B68" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>AA16:AC16</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B25" xr:uid="{00000000-0002-0000-0800-000001000000}">
       <formula1>AA25:AD25</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B30">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B30" xr:uid="{00000000-0002-0000-0800-000002000000}">
       <formula1>AA30:AH30</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B35" xr:uid="{00000000-0002-0000-0800-000003000000}">
       <formula1>AA35:AF35</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B43">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B43" xr:uid="{00000000-0002-0000-0800-000004000000}">
       <formula1>AA43:AE43</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B55">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B55 B76" xr:uid="{00000000-0002-0000-0800-000005000000}">
       <formula1>AA55:AB55</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B63">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B63 B84" xr:uid="{00000000-0002-0000-0800-000006000000}">
       <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B68">
-      <formula1>AA68:AC68</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B76">
-      <formula1>AA76:AB76</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B84">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B89">
-      <formula1>AA89:AC89</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated Toplevel, Atmos for NICAM16-9s, and responsible_parties.
</commit_message>
<xml_diff>
--- a/cmip6/models/nicam16-9s/cmip6_miroc_nicam16-9s_atmos.xlsx
+++ b/cmip6/models/nicam16-9s/cmip6_miroc_nicam16-9s_atmos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\kodama_home\研究\CMIP\CMIP6\ES-DOC\03.とりまとめ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C4DB9E-5908-4155-90E8-09B1B276535F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8FE678-63EB-4009-B1C5-4319A6BDE999}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="14616" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10440" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" r:id="rId1"/>
@@ -26,12 +26,20 @@
     <sheet name="9. Gravity Waves" sheetId="11" r:id="rId11"/>
     <sheet name="10. Natural Forcing" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1672" uniqueCount="1105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1991" uniqueCount="1149">
   <si>
     <t>ES-DOC CMIP6 Model Documentation</t>
   </si>
@@ -3312,10 +3320,6 @@
     <phoneticPr fontId="15"/>
   </si>
   <si>
-    <t>non-hydrostatic model, icosahedral grid, explicit convection</t>
-    <phoneticPr fontId="15"/>
-  </si>
-  <si>
     <t xml:space="preserve">NICAM is a Nonhydrostatic ICosahedral Atmospheric Model (NICAM), used as a Global Cloud Resolving Model (GCRM). A subkilometer-mesh global simulation is already performed using the K computer by Miyamoto et al. (2013). NICAM is first developed by H.Tomita (JAMSTEC; now at AICS, RIKEN) and M.Satoh (AORI, The Univ. of Tokyo), and is now under development in cooperation with AORI, JAMSTEC, and RIKEN by the NICAM developers listed on http://nicam.jp/. Introduction papers of NICAM are Satoh et al. (2014, PEPS), Satoh et al.(2008, J.Comp. Physics), and Tomita and Satoh (2004, Fluid Dyn. Res.). </t>
     <phoneticPr fontId="15"/>
   </si>
@@ -3324,48 +3328,209 @@
     <phoneticPr fontId="15"/>
   </si>
   <si>
-    <t>14km lat-lon</t>
+    <t>Zonal mean zonal wind, surface air temperature</t>
     <phoneticPr fontId="15"/>
   </si>
   <si>
-    <t>14km</t>
+    <t>NICAM uses an icosahedral grid. Higher resolution grids are recursively subdivided from a coarser resolution grid. See Satoh et al. (2014) for details</t>
     <phoneticPr fontId="15"/>
   </si>
   <si>
-    <t xml:space="preserve">Cloud microphysics scheme were constrained using TRMM satellite in process-oriented manner. Zonal mean zonal wind, specifically, location of midlatitude jet was used as a metric to tune the wave generation parameter in orographic gravity wave drag scheme. Surface air temperature was monitored to tune a parameter to diagnose sea ice thickness from sea ice concentration. OLR (clear &amp; cloudy), OSR (clear &amp; cloudy), precipitation and cloud fraction were often checked, though they were not a direct target of tuning this time.
+    <t>None</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>McFarlane</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>Conventional ogographic gravity wave drag scheme by McFarlane (1987)</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>Proportional to sub-grid scale orography variance, stability and surface wind</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>NSW6</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t xml:space="preserve">NSW6 is a single-moment bulk cloud microphysics scheme with six water categories (water vapor, cloud water, rain, cloud ice, snow, and graupel). The mass concentration of the water categories are predicted and thermodynamics are solved to conserve of mass and moist-internal energy. Hydrometeors' tendencies are derived by integrating growth equations of a hydrometeor particle with the particle size distribution. Graviational sedimentation is solved using a semi-Lagrangian scheme, which is conservative and positive-definite. </t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>Liquid rain</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t xml:space="preserve">NICAM is a cloud resolving model and, hence, cloud fraction is assumed to be unity or zero. </t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>Cloud fraction is not used</t>
+  </si>
+  <si>
+    <t>Cloud fraction is not used</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>Only microphysics scheme is used</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>Graupel</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>Atmosphere_turbulence_convection</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>Grid-resolved cloud</t>
+  </si>
+  <si>
+    <t>Grid-resolved cloud</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>Kodama</t>
+  </si>
+  <si>
+    <t>Point of Contact</t>
+  </si>
+  <si>
+    <t>Ohno</t>
+  </si>
+  <si>
+    <t>Contributor</t>
+  </si>
+  <si>
+    <t>Seiki</t>
+  </si>
+  <si>
+    <t>Yashiro</t>
+  </si>
+  <si>
+    <t>Noda</t>
+  </si>
+  <si>
+    <t>Nakano</t>
+  </si>
+  <si>
+    <t>Yamada</t>
+  </si>
+  <si>
+    <t>Roh</t>
+  </si>
+  <si>
+    <t>Satoh</t>
+  </si>
+  <si>
+    <t>Nitta</t>
+  </si>
+  <si>
+    <t>Nasuno</t>
+  </si>
+  <si>
+    <t>Miyakawa</t>
+  </si>
+  <si>
+    <t>Chen</t>
+  </si>
+  <si>
+    <t>Sugi</t>
+  </si>
+  <si>
+    <t>non-hydrostatic model, icosahedral grid, cloud-resolving model</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>14 km lat-lon</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>14 km</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloud microphysics scheme were constrained using TRMM satellite in process-oriented manner (Roh and Satoh 2014). Zonal mean zonal wind, specifically, location of midlatitude jet was used as a metric to tune the wave generation parameter in orographic gravity wave drag scheme. Surface air temperature was monitored to tune a parameter to diagnose sea ice thickness from sea ice concentration. OLR (clear &amp; cloudy), OSR (clear &amp; cloudy), precipitation and cloud fraction were checked, though they were not a direct target of tuning this time.
 </t>
     <phoneticPr fontId="15"/>
   </si>
   <si>
-    <t>Zonal mean zonal wind, surface air temperature</t>
+    <t xml:space="preserve"> </t>
     <phoneticPr fontId="15"/>
   </si>
   <si>
-    <t>icosahedral grid</t>
+    <t>Note: unit in GHz</t>
     <phoneticPr fontId="15"/>
   </si>
   <si>
-    <t>NICAM uses an icosahedral grid. Higher resolution grids are recursively subdivided from a coarser resolution grid. See Satoh et al. (2014) for details</t>
+    <t>Max/Random</t>
     <phoneticPr fontId="15"/>
   </si>
   <si>
-    <t>None</t>
+    <t>Extinction factor, single-scattering albedo, and asymmetry factor are considered for each band in the radiation scheme above the tropopause.</t>
     <phoneticPr fontId="15"/>
   </si>
   <si>
-    <t>McFarlane</t>
+    <t>Icosahedral grid</t>
     <phoneticPr fontId="15"/>
   </si>
   <si>
-    <t>Conventional ogographic gravity wave drag scheme by McFarlane (1987)</t>
+    <t>Other: document in cell to the right</t>
     <phoneticPr fontId="15"/>
   </si>
   <si>
-    <t>Proportional to sub-grid scale orography variance, stability and surface wind</t>
+    <t>No pole singularity. The pole point is treated as a grid point</t>
     <phoneticPr fontId="15"/>
   </si>
   <si>
-    <t>Above the tropopause, extinction factor, single-scattering albedo, and asymmetry factor are considered for each band in the radiation scheme</t>
+    <t>Terrain-following, height coordinate</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>NICAM-DC</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>The fully compressive equation system is discretized by a finite volume mothod on the global icosahedral grid system. The numerical method is based on the conservative scheme for mass and total energy. The time-splitting (split-explicit) scheme is used in the horizontal directions by decomposing the fast and slow mode terms. In the small time step, the set of equation is solved explicitly in the horizontal directions and implicitly in the vertical direction (HE-VI). The advection scheme is an upwind bias scheme, considered the consistency with continuity (CWC). See Tomita and Satoh (2004), Satoh et al. (2008), and Satoh et al. (2014) for details.</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>Wicker and Skamarock (2002)</t>
+  </si>
+  <si>
+    <t>density</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>total internal energy</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>Neumann boundary condition, non-gradient</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>Free-slip, rigid surface condition for the horizontal verocity.  The vertical velocity is assumed to be zero.</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>Biharmonaic diffusion (Satoh et al., 2008)</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>Miura (2007); Niwa et al. (2011a)</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>Eulerian</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>Finite volume method</t>
     <phoneticPr fontId="15"/>
   </si>
 </sst>
@@ -4069,9 +4234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AD78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15"/>
   <cols>
@@ -4394,14 +4557,19 @@
       </c>
     </row>
     <row r="53" spans="1:29" ht="24" customHeight="1">
-      <c r="B53" s="11"/>
+      <c r="B53" s="11">
+        <v>94</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>1131</v>
+      </c>
     </row>
     <row r="55" spans="1:29" ht="24" customHeight="1">
       <c r="A55" s="9" t="s">
         <v>895</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>121</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="56" spans="1:29" ht="24" customHeight="1">
@@ -4416,7 +4584,9 @@
       </c>
     </row>
     <row r="57" spans="1:29" ht="24" customHeight="1">
-      <c r="B57" s="11"/>
+      <c r="B57" s="11" t="s">
+        <v>899</v>
+      </c>
       <c r="AA57" s="6" t="s">
         <v>898</v>
       </c>
@@ -4447,7 +4617,9 @@
       </c>
     </row>
     <row r="61" spans="1:29" ht="24" customHeight="1">
-      <c r="B61" s="11"/>
+      <c r="B61" s="11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="63" spans="1:29" ht="24" customHeight="1">
       <c r="A63" s="9" t="s">
@@ -4469,7 +4641,9 @@
       </c>
     </row>
     <row r="65" spans="1:29" ht="24" customHeight="1">
-      <c r="B65" s="11"/>
+      <c r="B65" s="11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="68" spans="1:29" ht="24" customHeight="1">
       <c r="A68" s="12" t="s">
@@ -4504,7 +4678,9 @@
       </c>
     </row>
     <row r="73" spans="1:29" ht="24" customHeight="1">
-      <c r="B73" s="11"/>
+      <c r="B73" s="11" t="s">
+        <v>915</v>
+      </c>
       <c r="AA73" s="6" t="s">
         <v>915</v>
       </c>
@@ -4540,7 +4716,12 @@
       </c>
     </row>
     <row r="78" spans="1:29" ht="24" customHeight="1">
-      <c r="B78" s="11"/>
+      <c r="B78" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>1132</v>
+      </c>
       <c r="AA78" s="6" t="s">
         <v>921</v>
       </c>
@@ -4579,8 +4760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AF76"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+    <sheetView topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15"/>
@@ -4625,7 +4806,7 @@
     </row>
     <row r="6" spans="1:29" ht="24" customHeight="1">
       <c r="B6" s="11" t="s">
-        <v>1101</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="24" customHeight="1">
@@ -4654,7 +4835,7 @@
     </row>
     <row r="11" spans="1:29" ht="178.05" customHeight="1">
       <c r="B11" s="11" t="s">
-        <v>1102</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="13" spans="1:29" ht="24" customHeight="1">
@@ -4798,7 +4979,7 @@
     </row>
     <row r="32" spans="1:30" ht="24" customHeight="1">
       <c r="B32" s="11" t="s">
-        <v>1101</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="34" spans="1:32" ht="24" customHeight="1">
@@ -4877,7 +5058,7 @@
         <v>66</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>1103</v>
+        <v>1098</v>
       </c>
       <c r="AA42" s="6" t="s">
         <v>969</v>
@@ -5001,7 +5182,7 @@
     </row>
     <row r="58" spans="1:32" ht="24" customHeight="1">
       <c r="B58" s="11" t="s">
-        <v>1100</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="60" spans="1:32" ht="24" customHeight="1">
@@ -5185,9 +5366,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:AD77"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15"/>
   <cols>
@@ -5594,7 +5773,7 @@
     </row>
     <row r="73" spans="1:29" ht="178.05" customHeight="1">
       <c r="B73" s="11" t="s">
-        <v>1104</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="75" spans="1:29" ht="24" customHeight="1">
@@ -5660,9 +5839,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15"/>
   <cols>
@@ -5707,50 +5888,158 @@
       </c>
     </row>
     <row r="9" spans="1:2" ht="17.399999999999999">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
+      <c r="A9" s="11" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="17.399999999999999">
+      <c r="A10" s="11" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="17.399999999999999">
+      <c r="A11" s="11" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>1113</v>
+      </c>
     </row>
     <row r="12" spans="1:2" ht="17.399999999999999">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="11" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="17.399999999999999">
+      <c r="A13" s="11" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="17.399999999999999">
+      <c r="A14" s="11" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="17.399999999999999">
+      <c r="A15" s="11" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="17.399999999999999">
+      <c r="A16" s="11" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="17.399999999999999">
+      <c r="A17" s="11" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="17.399999999999999">
+      <c r="A18" s="11" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="17.399999999999999">
+      <c r="A19" s="11" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="17.399999999999999">
+      <c r="A20" s="11" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="17.399999999999999">
+      <c r="A21" s="11" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="17.399999999999999">
+      <c r="A22" s="11" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="17.399999999999999">
+      <c r="A25" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="9"/>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="8" t="s">
+      <c r="B25" s="9"/>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="8" t="s">
+    <row r="28" spans="1:2">
+      <c r="A28" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15.6">
-      <c r="A16" s="10" t="s">
+    <row r="29" spans="1:2" ht="15.6">
+      <c r="A29" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B29" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="17.399999999999999">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
+    <row r="30" spans="1:2" ht="17.399999999999999">
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="15"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:B22" xr:uid="{00AE6EB9-842D-4EDC-9683-9C795DBEF2C4}">
       <formula1>"Author,Contributor,Principal Investigator,Point of Contact,Sponsor"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17" xr:uid="{00000000-0002-0000-0100-000001000000}">
-      <formula1>"Top Level,Key Properties,Grid,Dynamical Core,Radiation,Turbulence Convection,Microphysics Precipitation,Cloud Scheme,Observation Simulation,Gravity Waves,Natural Forcing"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B30" xr:uid="{98B065E9-B594-4167-BC71-0BECBF41A4DA}">
+      <formula1>"Top Level,Key Properties,Radiative Forcings"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="A13" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="A6" r:id="rId1" xr:uid="{91A21BE9-6157-4156-949F-F5829DE9477D}"/>
+    <hyperlink ref="A26" r:id="rId2" xr:uid="{961A653C-4936-4705-B459-60C6BCC8A5B1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5760,8 +6049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AG106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15"/>
@@ -5835,7 +6124,7 @@
     </row>
     <row r="11" spans="1:3" ht="24" customHeight="1">
       <c r="B11" s="11" t="s">
-        <v>1091</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="24" customHeight="1">
@@ -5864,7 +6153,7 @@
     </row>
     <row r="16" spans="1:3" ht="178.05" customHeight="1">
       <c r="B16" s="11" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="18" spans="1:33" ht="24" customHeight="1">
@@ -5984,7 +6273,7 @@
     </row>
     <row r="33" spans="1:3" ht="24" customHeight="1">
       <c r="B33" s="11" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="24" customHeight="1">
@@ -6008,7 +6297,7 @@
     </row>
     <row r="37" spans="1:3" ht="24" customHeight="1">
       <c r="B37" s="11" t="s">
-        <v>1094</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="24" customHeight="1">
@@ -6032,7 +6321,7 @@
     </row>
     <row r="41" spans="1:3" ht="24" customHeight="1">
       <c r="B41" s="11" t="s">
-        <v>1095</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="24" customHeight="1">
@@ -6317,7 +6606,7 @@
     </row>
     <row r="91" spans="1:3" ht="178.05" customHeight="1">
       <c r="B91" s="11" t="s">
-        <v>1096</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="24" customHeight="1">
@@ -6346,7 +6635,7 @@
     </row>
     <row r="96" spans="1:3" ht="24" customHeight="1">
       <c r="B96" s="11" t="s">
-        <v>1097</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="24" customHeight="1">
@@ -6427,6 +6716,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6434,8 +6724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AF44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15"/>
@@ -6480,7 +6770,7 @@
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1">
       <c r="B6" s="11" t="s">
-        <v>1098</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1">
@@ -6509,7 +6799,7 @@
     </row>
     <row r="11" spans="1:3" ht="178.05" customHeight="1">
       <c r="B11" s="11" t="s">
-        <v>1099</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
@@ -6545,7 +6835,9 @@
       </c>
     </row>
     <row r="19" spans="1:30" ht="24" customHeight="1">
-      <c r="B19" s="11"/>
+      <c r="B19" s="11" t="s">
+        <v>174</v>
+      </c>
       <c r="AA19" s="6" t="s">
         <v>173</v>
       </c>
@@ -6576,7 +6868,9 @@
       </c>
     </row>
     <row r="23" spans="1:30" ht="24" customHeight="1">
-      <c r="B23" s="11"/>
+      <c r="B23" s="11" t="s">
+        <v>180</v>
+      </c>
       <c r="AA23" s="6" t="s">
         <v>179</v>
       </c>
@@ -6610,7 +6904,9 @@
       </c>
     </row>
     <row r="27" spans="1:30" ht="24" customHeight="1">
-      <c r="B27" s="11"/>
+      <c r="B27" s="11" t="s">
+        <v>187</v>
+      </c>
       <c r="AA27" s="6" t="s">
         <v>187</v>
       </c>
@@ -6644,7 +6940,12 @@
       </c>
     </row>
     <row r="31" spans="1:30" ht="24" customHeight="1">
-      <c r="B31" s="11"/>
+      <c r="B31" s="11" t="s">
+        <v>1135</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>1136</v>
+      </c>
       <c r="AA31" s="6" t="s">
         <v>194</v>
       </c>
@@ -6678,7 +6979,9 @@
       </c>
     </row>
     <row r="35" spans="1:32" ht="24" customHeight="1">
-      <c r="B35" s="11"/>
+      <c r="B35" s="11" t="s">
+        <v>204</v>
+      </c>
       <c r="AA35" s="6" t="s">
         <v>201</v>
       </c>
@@ -6733,7 +7036,12 @@
       </c>
     </row>
     <row r="44" spans="1:32" ht="24" customHeight="1">
-      <c r="B44" s="11"/>
+      <c r="B44" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>1137</v>
+      </c>
       <c r="AA44" s="6" t="s">
         <v>212</v>
       </c>
@@ -6756,16 +7064,16 @@
   </sheetData>
   <phoneticPr fontId="15"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19" xr:uid="{1B737186-00E8-49B2-9659-D2C3F31C62B2}">
       <formula1>AA19:AC19</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23 B31 B27" xr:uid="{00000000-0002-0000-0300-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23 B31 B27" xr:uid="{61B37808-2EE3-45E2-866C-99D0B9585339}">
       <formula1>AA23:AD23</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B35" xr:uid="{00000000-0002-0000-0300-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B35" xr:uid="{D2AE134A-EBFD-41D5-A912-41FC23BAB1C6}">
       <formula1>AA35:AE35</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B44" xr:uid="{00000000-0002-0000-0300-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B44" xr:uid="{BB5DD873-5256-4E46-900A-8B8BF8D20C74}">
       <formula1>AA44:AF44</formula1>
     </dataValidation>
   </dataValidations>
@@ -6775,9 +7083,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:AM104"/>
+  <dimension ref="A1:AM114"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15"/>
   <cols>
@@ -6820,7 +7128,9 @@
       </c>
     </row>
     <row r="6" spans="1:36" ht="24" customHeight="1">
-      <c r="B6" s="11"/>
+      <c r="B6" s="11" t="s">
+        <v>1138</v>
+      </c>
     </row>
     <row r="8" spans="1:36" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
@@ -6847,7 +7157,9 @@
       </c>
     </row>
     <row r="11" spans="1:36" ht="178.05" customHeight="1">
-      <c r="B11" s="11"/>
+      <c r="B11" s="11" t="s">
+        <v>1139</v>
+      </c>
     </row>
     <row r="13" spans="1:36" ht="24" customHeight="1">
       <c r="A13" s="9" t="s">
@@ -6869,7 +7181,12 @@
       </c>
     </row>
     <row r="15" spans="1:36" ht="24" customHeight="1">
-      <c r="B15" s="11"/>
+      <c r="B15" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>1140</v>
+      </c>
       <c r="AA15" s="6" t="s">
         <v>230</v>
       </c>
@@ -6926,7 +7243,9 @@
       </c>
     </row>
     <row r="20" spans="1:39" ht="24" customHeight="1">
-      <c r="B20" s="11"/>
+      <c r="B20" s="11" t="s">
+        <v>244</v>
+      </c>
       <c r="AA20" s="6" t="s">
         <v>243</v>
       </c>
@@ -6967,329 +7286,512 @@
         <v>66</v>
       </c>
     </row>
+    <row r="21" spans="1:39" ht="24" customHeight="1">
+      <c r="B21" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>1141</v>
+      </c>
+      <c r="AA21" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="AB21" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="AC21" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="AD21" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="AE21" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="AF21" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="AG21" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="AH21" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="AI21" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="AJ21" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="AK21" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="AL21" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="AM21" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:39" ht="24" customHeight="1">
+      <c r="B22" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>1142</v>
+      </c>
+      <c r="AA22" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="AB22" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="AC22" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="AD22" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="AE22" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="AF22" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="AG22" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="AH22" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="AI22" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="AJ22" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="AK22" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="AL22" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="AM22" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
     <row r="23" spans="1:39" ht="24" customHeight="1">
-      <c r="A23" s="12" t="s">
+      <c r="B23" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="AA23" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="AB23" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="AC23" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="AD23" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="AE23" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="AF23" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="AG23" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="AH23" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="AI23" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="AJ23" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="AK23" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="AL23" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="AM23" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:39" ht="24" customHeight="1">
+      <c r="B24" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="AA24" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="AB24" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="AC24" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="AD24" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="AE24" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="AF24" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="AG24" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="AH24" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="AI24" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="AJ24" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="AK24" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="AL24" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="AM24" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:39" ht="24" customHeight="1">
+      <c r="B25" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="AA25" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="AB25" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="AC25" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="AD25" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="AE25" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="AF25" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="AG25" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="AH25" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="AI25" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="AJ25" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="AK25" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="AL25" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="AM25" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:39" ht="24" customHeight="1">
+      <c r="A28" s="12" t="s">
         <v>255</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B28" s="12" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="24" spans="1:39" ht="24" customHeight="1">
-      <c r="B24" s="13" t="s">
+    <row r="29" spans="1:39" ht="24" customHeight="1">
+      <c r="B29" s="13" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="26" spans="1:39" ht="24" customHeight="1">
-      <c r="A26" s="9" t="s">
+    <row r="31" spans="1:39" ht="24" customHeight="1">
+      <c r="A31" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B31" s="9" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="27" spans="1:39" ht="24" customHeight="1">
-      <c r="A27" s="14" t="s">
+    <row r="32" spans="1:39" ht="24" customHeight="1">
+      <c r="A32" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B32" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C32" s="10" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="28" spans="1:39" ht="24" customHeight="1">
-      <c r="B28" s="11"/>
-      <c r="AA28" s="6" t="s">
+    <row r="33" spans="1:29" ht="24" customHeight="1">
+      <c r="B33" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="AB28" s="6" t="s">
+      <c r="AA33" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="AB33" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="AC28" s="6" t="s">
+      <c r="AC33" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:39" ht="24" customHeight="1">
-      <c r="A30" s="9" t="s">
+    <row r="34" spans="1:29" ht="24" customHeight="1"/>
+    <row r="35" spans="1:29" ht="24" customHeight="1">
+      <c r="A35" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B35" s="9" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="31" spans="1:39" ht="24" customHeight="1">
-      <c r="A31" s="14" t="s">
+    <row r="36" spans="1:29" ht="24" customHeight="1">
+      <c r="A36" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B36" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C36" s="10" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="32" spans="1:39" ht="24" customHeight="1">
-      <c r="B32" s="11"/>
-    </row>
-    <row r="34" spans="1:29" ht="24" customHeight="1">
-      <c r="A34" s="9" t="s">
+    <row r="37" spans="1:29" ht="24" customHeight="1">
+      <c r="B37" s="11" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="39" spans="1:29" ht="24" customHeight="1">
+      <c r="A39" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B39" s="9" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="35" spans="1:29" ht="24" customHeight="1">
-      <c r="A35" s="14" t="s">
+    <row r="40" spans="1:29" ht="24" customHeight="1">
+      <c r="A40" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B40" s="10" t="s">
         <v>270</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C40" s="10" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="36" spans="1:29" ht="24" customHeight="1">
-      <c r="B36" s="11"/>
-    </row>
-    <row r="39" spans="1:29" ht="24" customHeight="1">
-      <c r="A39" s="12" t="s">
+    <row r="41" spans="1:29" ht="24" customHeight="1">
+      <c r="B41" s="11" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="42" spans="1:29" ht="24" customHeight="1"/>
+    <row r="43" spans="1:29" ht="24" customHeight="1"/>
+    <row r="44" spans="1:29" ht="24" customHeight="1">
+      <c r="A44" s="12" t="s">
         <v>272</v>
       </c>
-      <c r="B39" s="12" t="s">
+      <c r="B44" s="12" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="40" spans="1:29" ht="24" customHeight="1">
-      <c r="B40" s="13" t="s">
+    <row r="45" spans="1:29" ht="24" customHeight="1">
+      <c r="B45" s="13" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="42" spans="1:29" ht="24" customHeight="1">
-      <c r="A42" s="9" t="s">
+    <row r="47" spans="1:29" ht="24" customHeight="1">
+      <c r="A47" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B47" s="9" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="43" spans="1:29" ht="24" customHeight="1">
-      <c r="A43" s="14" t="s">
+    <row r="48" spans="1:29" ht="24" customHeight="1">
+      <c r="A48" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B48" s="10" t="s">
         <v>277</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C48" s="10" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="44" spans="1:29" ht="24" customHeight="1">
-      <c r="B44" s="11"/>
-      <c r="AA44" s="6" t="s">
+    <row r="49" spans="1:29" ht="24" customHeight="1">
+      <c r="B49" s="11"/>
+      <c r="AA49" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="AB44" s="6" t="s">
+      <c r="AB49" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="AC44" s="6" t="s">
+      <c r="AC49" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="47" spans="1:29" ht="24" customHeight="1">
-      <c r="A47" s="12" t="s">
+    <row r="50" spans="1:29" ht="24" customHeight="1"/>
+    <row r="51" spans="1:29" ht="24" customHeight="1"/>
+    <row r="52" spans="1:29" ht="24" customHeight="1">
+      <c r="A52" s="12" t="s">
         <v>279</v>
       </c>
-      <c r="B47" s="12" t="s">
+      <c r="B52" s="12" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="48" spans="1:29" ht="24" customHeight="1">
-      <c r="B48" s="13" t="s">
+    <row r="53" spans="1:29" ht="24" customHeight="1">
+      <c r="B53" s="13" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="50" spans="1:32" ht="24" customHeight="1">
-      <c r="A50" s="9" t="s">
+    <row r="54" spans="1:29" ht="24" customHeight="1"/>
+    <row r="55" spans="1:29" ht="24" customHeight="1">
+      <c r="A55" s="9" t="s">
         <v>282</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="B55" s="9" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="51" spans="1:32" ht="24" customHeight="1">
-      <c r="A51" s="14" t="s">
+    <row r="56" spans="1:29" ht="24" customHeight="1">
+      <c r="A56" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B51" s="10" t="s">
+      <c r="B56" s="10" t="s">
         <v>284</v>
       </c>
-      <c r="C51" s="10" t="s">
+      <c r="C56" s="10" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="52" spans="1:32" ht="24" customHeight="1">
-      <c r="B52" s="11"/>
-    </row>
-    <row r="54" spans="1:32" ht="24" customHeight="1">
-      <c r="A54" s="9" t="s">
+    <row r="57" spans="1:29" ht="24" customHeight="1">
+      <c r="B57" s="11" t="s">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="59" spans="1:29" ht="24" customHeight="1">
+      <c r="A59" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="B54" s="9" t="s">
+      <c r="B59" s="9" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="55" spans="1:32" ht="24" customHeight="1">
-      <c r="A55" s="14" t="s">
+    <row r="60" spans="1:29" ht="24" customHeight="1">
+      <c r="A60" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="B55" s="10" t="s">
+      <c r="B60" s="10" t="s">
         <v>287</v>
       </c>
-      <c r="C55" s="10" t="s">
+      <c r="C60" s="10" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="56" spans="1:32" ht="24" customHeight="1">
-      <c r="B56" s="11"/>
-      <c r="AA56" s="6" t="s">
+    <row r="61" spans="1:29" ht="24" customHeight="1">
+      <c r="B61" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="AA61" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="AB56" s="6" t="s">
+      <c r="AB61" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="AC56" s="6" t="s">
+      <c r="AC61" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="59" spans="1:32" ht="24" customHeight="1">
-      <c r="A59" s="12" t="s">
+    <row r="62" spans="1:29" ht="24" customHeight="1"/>
+    <row r="63" spans="1:29" ht="24" customHeight="1"/>
+    <row r="64" spans="1:29" ht="24" customHeight="1">
+      <c r="A64" s="12" t="s">
         <v>291</v>
       </c>
-      <c r="B59" s="12" t="s">
+      <c r="B64" s="12" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="60" spans="1:32" ht="24" customHeight="1">
-      <c r="B60" s="13" t="s">
+    <row r="65" spans="1:39" ht="24" customHeight="1">
+      <c r="B65" s="13" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="62" spans="1:32" ht="24" customHeight="1">
-      <c r="A62" s="9" t="s">
+    <row r="67" spans="1:39" ht="24" customHeight="1">
+      <c r="A67" s="9" t="s">
         <v>294</v>
       </c>
-      <c r="B62" s="9" t="s">
+      <c r="B67" s="9" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="63" spans="1:32" ht="24" customHeight="1">
-      <c r="A63" s="14" t="s">
+    <row r="68" spans="1:39" ht="24" customHeight="1">
+      <c r="A68" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="B63" s="10" t="s">
+      <c r="B68" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="C63" s="10" t="s">
+      <c r="C68" s="10" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="64" spans="1:32" ht="24" customHeight="1">
-      <c r="B64" s="11"/>
-      <c r="AA64" s="6" t="s">
+    <row r="69" spans="1:39" ht="24" customHeight="1">
+      <c r="B69" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>1146</v>
+      </c>
+      <c r="AA69" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="AB64" s="6" t="s">
+      <c r="AB69" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="AC64" s="6" t="s">
+      <c r="AC69" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="AD64" s="6" t="s">
+      <c r="AD69" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="AE64" s="6" t="s">
+      <c r="AE69" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="AF64" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="66" spans="1:39" ht="24" customHeight="1">
-      <c r="A66" s="9" t="s">
-        <v>302</v>
-      </c>
-      <c r="B66" s="9" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="67" spans="1:39" ht="24" customHeight="1">
-      <c r="A67" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B67" s="10" t="s">
-        <v>304</v>
-      </c>
-      <c r="C67" s="10" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="68" spans="1:39" ht="24" customHeight="1">
-      <c r="B68" s="10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="69" spans="1:39" ht="24" customHeight="1">
-      <c r="B69" s="11"/>
-      <c r="AA69" s="6" t="s">
-        <v>306</v>
-      </c>
-      <c r="AB69" s="6" t="s">
-        <v>307</v>
-      </c>
-      <c r="AC69" s="6" t="s">
-        <v>308</v>
-      </c>
-      <c r="AD69" s="6" t="s">
-        <v>309</v>
-      </c>
-      <c r="AE69" s="6" t="s">
-        <v>310</v>
-      </c>
       <c r="AF69" s="6" t="s">
-        <v>311</v>
-      </c>
-      <c r="AG69" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="AH69" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="AI69" s="6" t="s">
-        <v>314</v>
-      </c>
-      <c r="AJ69" s="6" t="s">
-        <v>315</v>
-      </c>
-      <c r="AK69" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="AL69" s="6" t="s">
-        <v>317</v>
-      </c>
-      <c r="AM69" s="6" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="71" spans="1:39" ht="24" customHeight="1">
       <c r="A71" s="9" t="s">
-        <v>318</v>
+        <v>302</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>319</v>
+        <v>303</v>
       </c>
     </row>
     <row r="72" spans="1:39" ht="24" customHeight="1">
@@ -7297,10 +7799,10 @@
         <v>61</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>320</v>
+        <v>304</v>
       </c>
       <c r="C72" s="10" t="s">
-        <v>321</v>
+        <v>305</v>
       </c>
     </row>
     <row r="73" spans="1:39" ht="24" customHeight="1">
@@ -7309,231 +7811,356 @@
       </c>
     </row>
     <row r="74" spans="1:39" ht="24" customHeight="1">
-      <c r="B74" s="11"/>
+      <c r="B74" s="11" t="s">
+        <v>1147</v>
+      </c>
       <c r="AA74" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="AB74" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="AC74" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="AD74" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="AE74" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="AF74" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="AG74" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="AH74" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="AI74" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="AJ74" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="AK74" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="AL74" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="AM74" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="75" spans="1:39" ht="24" customHeight="1">
+      <c r="B75" s="11" t="s">
+        <v>314</v>
+      </c>
+      <c r="AA75" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="AB75" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="AC75" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="AD75" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="AE75" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="AF75" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="AG75" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="AH75" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="AI75" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="AJ75" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="AK75" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="AL75" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="AM75" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="76" spans="1:39" ht="24" customHeight="1">
+      <c r="B76" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="AA76" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="AB76" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="AC76" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="AD76" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="AE76" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="AF76" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="AG76" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="AH76" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="AI76" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="AJ76" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="AK76" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="AL76" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="AM76" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="78" spans="1:39" ht="24" customHeight="1">
+      <c r="A78" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="B78" s="9" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="79" spans="1:39" ht="24" customHeight="1">
+      <c r="A79" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B79" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="C79" s="10" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="80" spans="1:39" ht="24" customHeight="1">
+      <c r="B80" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="81" spans="1:30" ht="24" customHeight="1">
+      <c r="B81" s="11" t="s">
         <v>322</v>
       </c>
-      <c r="AB74" s="6" t="s">
+      <c r="AA81" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="AB81" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="AC74" s="6" t="s">
+      <c r="AC81" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="76" spans="1:39" ht="24" customHeight="1">
-      <c r="A76" s="9" t="s">
+    <row r="82" spans="1:30" ht="24" customHeight="1">
+      <c r="B82" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="AA82" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="AB82" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="AC82" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="84" spans="1:30" ht="24" customHeight="1">
+      <c r="A84" s="9" t="s">
         <v>324</v>
       </c>
-      <c r="B76" s="9" t="s">
+      <c r="B84" s="9" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="77" spans="1:39" ht="24" customHeight="1">
-      <c r="A77" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B77" s="10" t="s">
-        <v>326</v>
-      </c>
-      <c r="C77" s="10" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="78" spans="1:39" ht="24" customHeight="1">
-      <c r="B78" s="11"/>
-      <c r="AA78" s="6" t="s">
-        <v>328</v>
-      </c>
-      <c r="AB78" s="6" t="s">
-        <v>329</v>
-      </c>
-      <c r="AC78" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="81" spans="1:32" ht="24" customHeight="1">
-      <c r="A81" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="B81" s="12" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="82" spans="1:32" ht="24" customHeight="1">
-      <c r="B82" s="13" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="84" spans="1:32" ht="24" customHeight="1">
-      <c r="A84" s="9" t="s">
-        <v>333</v>
-      </c>
-      <c r="B84" s="9" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="85" spans="1:32" ht="24" customHeight="1">
+    <row r="85" spans="1:30" ht="24" customHeight="1">
       <c r="A85" s="14" t="s">
         <v>61</v>
       </c>
       <c r="B85" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="C85" s="10" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="86" spans="1:30" ht="24" customHeight="1">
+      <c r="B86" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>1148</v>
+      </c>
+      <c r="AA86" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="AB86" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="AC86" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="88" spans="1:30" ht="24" customHeight="1"/>
+    <row r="89" spans="1:30" ht="24" customHeight="1">
+      <c r="A89" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="B89" s="12" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="90" spans="1:30" ht="24" customHeight="1">
+      <c r="B90" s="13" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="91" spans="1:30" ht="24" customHeight="1"/>
+    <row r="92" spans="1:30" ht="24" customHeight="1">
+      <c r="A92" s="9" t="s">
+        <v>333</v>
+      </c>
+      <c r="B92" s="9" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="93" spans="1:30" ht="24" customHeight="1">
+      <c r="A93" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B93" s="10" t="s">
         <v>334</v>
       </c>
-      <c r="C85" s="10" t="s">
+      <c r="C93" s="10" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="86" spans="1:32" ht="24" customHeight="1">
-      <c r="B86" s="11"/>
-      <c r="AA86" s="6" t="s">
+    <row r="94" spans="1:30" ht="24" customHeight="1">
+      <c r="B94" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D94" s="6" t="s">
+        <v>1148</v>
+      </c>
+      <c r="AA94" s="6" t="s">
         <v>336</v>
       </c>
-      <c r="AB86" s="6" t="s">
+      <c r="AB94" s="6" t="s">
         <v>337</v>
       </c>
-      <c r="AC86" s="6" t="s">
+      <c r="AC94" s="6" t="s">
         <v>338</v>
       </c>
-      <c r="AD86" s="6" t="s">
+      <c r="AD94" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="88" spans="1:32" ht="24" customHeight="1">
-      <c r="A88" s="9" t="s">
+    <row r="95" spans="1:30" ht="24" customHeight="1"/>
+    <row r="96" spans="1:30" ht="24" customHeight="1">
+      <c r="A96" s="9" t="s">
         <v>339</v>
       </c>
-      <c r="B88" s="9" t="s">
+      <c r="B96" s="9" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="89" spans="1:32" ht="24" customHeight="1">
-      <c r="A89" s="14" t="s">
+    <row r="97" spans="1:33" ht="24" customHeight="1">
+      <c r="A97" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="B89" s="10" t="s">
+      <c r="B97" s="10" t="s">
         <v>340</v>
       </c>
-      <c r="C89" s="10" t="s">
+      <c r="C97" s="10" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="90" spans="1:32" ht="24" customHeight="1">
-      <c r="B90" s="10" t="s">
+    <row r="98" spans="1:33" ht="24" customHeight="1">
+      <c r="B98" s="10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="91" spans="1:32" ht="24" customHeight="1">
-      <c r="B91" s="11"/>
-      <c r="AA91" s="6" t="s">
+    <row r="99" spans="1:33" ht="24" customHeight="1">
+      <c r="B99" s="11" t="s">
         <v>342</v>
       </c>
-      <c r="AB91" s="6" t="s">
+      <c r="AA99" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="AB99" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="AC91" s="6" t="s">
+      <c r="AC99" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="AD91" s="6" t="s">
+      <c r="AD99" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="AE91" s="6" t="s">
+      <c r="AE99" s="6" t="s">
         <v>346</v>
       </c>
-      <c r="AF91" s="6" t="s">
+      <c r="AF99" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="93" spans="1:32" ht="24" customHeight="1">
-      <c r="A93" s="9" t="s">
-        <v>347</v>
-      </c>
-      <c r="B93" s="9" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="94" spans="1:32" ht="24" customHeight="1">
-      <c r="A94" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B94" s="10" t="s">
-        <v>349</v>
-      </c>
-      <c r="C94" s="10" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="95" spans="1:32" ht="24" customHeight="1">
-      <c r="B95" s="11"/>
-      <c r="AA95" s="6" t="s">
-        <v>351</v>
-      </c>
-      <c r="AB95" s="6" t="s">
-        <v>352</v>
-      </c>
-      <c r="AC95" s="6" t="s">
-        <v>353</v>
-      </c>
-      <c r="AD95" s="6" t="s">
-        <v>354</v>
-      </c>
-      <c r="AE95" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="97" spans="1:33" ht="24" customHeight="1">
-      <c r="A97" s="9" t="s">
-        <v>355</v>
-      </c>
-      <c r="B97" s="9" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="98" spans="1:33" ht="24" customHeight="1">
-      <c r="A98" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B98" s="10" t="s">
-        <v>356</v>
-      </c>
-      <c r="C98" s="10" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="99" spans="1:33" ht="24" customHeight="1">
-      <c r="B99" s="10" t="s">
-        <v>31</v>
-      </c>
-    </row>
     <row r="100" spans="1:33" ht="24" customHeight="1">
-      <c r="B100" s="11"/>
+      <c r="B100" s="11" t="s">
+        <v>344</v>
+      </c>
       <c r="AA100" s="6" t="s">
-        <v>358</v>
+        <v>342</v>
       </c>
       <c r="AB100" s="6" t="s">
-        <v>359</v>
+        <v>343</v>
       </c>
       <c r="AC100" s="6" t="s">
-        <v>360</v>
+        <v>344</v>
       </c>
       <c r="AD100" s="6" t="s">
-        <v>361</v>
+        <v>345</v>
       </c>
       <c r="AE100" s="6" t="s">
-        <v>362</v>
+        <v>346</v>
       </c>
       <c r="AF100" s="6" t="s">
-        <v>363</v>
-      </c>
-      <c r="AG100" s="6" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="102" spans="1:33" ht="24" customHeight="1">
       <c r="A102" s="9" t="s">
-        <v>364</v>
+        <v>347</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>325</v>
+        <v>348</v>
       </c>
     </row>
     <row r="103" spans="1:33" ht="24" customHeight="1">
@@ -7541,47 +8168,165 @@
         <v>61</v>
       </c>
       <c r="B103" s="10" t="s">
-        <v>365</v>
+        <v>349</v>
       </c>
       <c r="C103" s="10" t="s">
-        <v>366</v>
+        <v>350</v>
       </c>
     </row>
     <row r="104" spans="1:33" ht="24" customHeight="1">
       <c r="B104" s="11"/>
       <c r="AA104" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="AB104" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="AC104" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="AD104" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="AE104" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="106" spans="1:33" ht="24" customHeight="1">
+      <c r="A106" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="B106" s="9" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="107" spans="1:33" ht="24" customHeight="1">
+      <c r="A107" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B107" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="C107" s="10" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="108" spans="1:33" ht="24" customHeight="1">
+      <c r="B108" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="109" spans="1:33" ht="24" customHeight="1">
+      <c r="B109" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="AA109" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="AB109" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="AC109" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="AD109" s="6" t="s">
+        <v>361</v>
+      </c>
+      <c r="AE109" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="AF109" s="6" t="s">
+        <v>363</v>
+      </c>
+      <c r="AG109" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="110" spans="1:33" ht="24" customHeight="1">
+      <c r="B110" s="11" t="s">
+        <v>362</v>
+      </c>
+      <c r="AA110" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="AB110" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="AC110" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="AD110" s="6" t="s">
+        <v>361</v>
+      </c>
+      <c r="AE110" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="AF110" s="6" t="s">
+        <v>363</v>
+      </c>
+      <c r="AG110" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="112" spans="1:33" ht="24" customHeight="1">
+      <c r="A112" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="B112" s="9" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="113" spans="1:28" ht="24" customHeight="1">
+      <c r="A113" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B113" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="C113" s="10" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="114" spans="1:28" ht="24" customHeight="1">
+      <c r="B114" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D114" s="6" t="s">
+        <v>1148</v>
+      </c>
+      <c r="AA114" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="AB104" s="6" t="s">
+      <c r="AB114" s="6" t="s">
         <v>66</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="15"/>
   <dataValidations count="8">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15" xr:uid="{8AFDA2F9-D99C-49EB-9F47-6ABB2611D1E4}">
       <formula1>AA15:AJ15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20 B69" xr:uid="{00000000-0002-0000-0400-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20:B25 B74:B76" xr:uid="{3640FA18-5026-456D-B553-FDA55E62CC39}">
       <formula1>AA20:AM20</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B28 B78 B74 B56 B44" xr:uid="{00000000-0002-0000-0400-000002000000}">
-      <formula1>AA28:AC28</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B33 B86 B81:B82 B61 B49" xr:uid="{BBB6A8D5-2DDB-4A85-A911-743467053CA5}">
+      <formula1>AA33:AC33</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B64 B91" xr:uid="{00000000-0002-0000-0400-000005000000}">
-      <formula1>AA64:AF64</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B69 B99:B100" xr:uid="{681EC51D-99D2-407A-81AB-FFC9CFED1DDD}">
+      <formula1>AA69:AF69</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B86" xr:uid="{00000000-0002-0000-0400-000009000000}">
-      <formula1>AA86:AD86</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B94" xr:uid="{F4A16A13-1B08-42AD-B4EA-E6895FAEFB72}">
+      <formula1>AA94:AD94</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B95" xr:uid="{00000000-0002-0000-0400-00000B000000}">
-      <formula1>AA95:AE95</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B104" xr:uid="{555A84D8-377A-472F-9831-71B4F7F79185}">
+      <formula1>AA104:AE104</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B100" xr:uid="{00000000-0002-0000-0400-00000C000000}">
-      <formula1>AA100:AG100</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B109:B110" xr:uid="{130C07A8-7194-4253-9358-A256F2FF9EB9}">
+      <formula1>AA109:AG109</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B104" xr:uid="{00000000-0002-0000-0400-00000D000000}">
-      <formula1>AA104:AB104</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B114" xr:uid="{F9309121-ABAA-48A1-A9EB-E6C626E3B0C2}">
+      <formula1>AA114:AB114</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7592,7 +8337,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AX206"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15"/>
   <cols>
@@ -9334,8 +10081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AK87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15"/>
@@ -10048,7 +10795,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:AI37"/>
+  <dimension ref="A1:AI45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -10093,7 +10840,9 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1">
-      <c r="B6" s="11"/>
+      <c r="B6" s="11" t="s">
+        <v>1099</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
@@ -10120,7 +10869,9 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="178.05" customHeight="1">
-      <c r="B11" s="11"/>
+      <c r="B11" s="11" t="s">
+        <v>1100</v>
+      </c>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
       <c r="A14" s="12" t="s">
@@ -10182,7 +10933,9 @@
       </c>
     </row>
     <row r="24" spans="1:31" ht="24" customHeight="1">
-      <c r="B24" s="11"/>
+      <c r="B24" s="11" t="s">
+        <v>1101</v>
+      </c>
       <c r="AA24" s="6" t="s">
         <v>731</v>
       </c>
@@ -10199,103 +10952,340 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:31" ht="24" customHeight="1">
-      <c r="A27" s="12" t="s">
+    <row r="25" spans="1:31" ht="24" customHeight="1">
+      <c r="B25" s="11" t="s">
+        <v>732</v>
+      </c>
+      <c r="AA25" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="AB25" s="6" t="s">
+        <v>732</v>
+      </c>
+      <c r="AC25" s="6" t="s">
+        <v>733</v>
+      </c>
+      <c r="AD25" s="6" t="s">
+        <v>734</v>
+      </c>
+      <c r="AE25" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" ht="24" customHeight="1">
+      <c r="B26" s="11" t="s">
+        <v>734</v>
+      </c>
+      <c r="AA26" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="AB26" s="6" t="s">
+        <v>732</v>
+      </c>
+      <c r="AC26" s="6" t="s">
+        <v>733</v>
+      </c>
+      <c r="AD26" s="6" t="s">
+        <v>734</v>
+      </c>
+      <c r="AE26" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" ht="24" customHeight="1"/>
+    <row r="28" spans="1:31" ht="24" customHeight="1"/>
+    <row r="29" spans="1:31" ht="24" customHeight="1">
+      <c r="A29" s="12" t="s">
         <v>735</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B29" s="12" t="s">
         <v>736</v>
       </c>
     </row>
-    <row r="28" spans="1:31" ht="24" customHeight="1">
-      <c r="B28" s="13" t="s">
+    <row r="30" spans="1:31" ht="24" customHeight="1">
+      <c r="B30" s="13" t="s">
         <v>737</v>
       </c>
     </row>
-    <row r="30" spans="1:31" ht="24" customHeight="1">
-      <c r="A30" s="9" t="s">
+    <row r="31" spans="1:31" ht="24" customHeight="1"/>
+    <row r="32" spans="1:31" ht="24" customHeight="1">
+      <c r="A32" s="9" t="s">
         <v>738</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B32" s="9" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="31" spans="1:31" ht="24" customHeight="1">
-      <c r="A31" s="14" t="s">
+    <row r="33" spans="1:35" ht="24" customHeight="1">
+      <c r="A33" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B33" s="10" t="s">
         <v>739</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C33" s="10" t="s">
         <v>740</v>
       </c>
     </row>
-    <row r="32" spans="1:31" ht="24" customHeight="1">
-      <c r="B32" s="11"/>
-    </row>
     <row r="34" spans="1:35" ht="24" customHeight="1">
-      <c r="A34" s="9" t="s">
+      <c r="B34" s="11"/>
+    </row>
+    <row r="36" spans="1:35" ht="24" customHeight="1">
+      <c r="A36" s="9" t="s">
         <v>741</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B36" s="9" t="s">
         <v>671</v>
       </c>
     </row>
-    <row r="35" spans="1:35" ht="24" customHeight="1">
-      <c r="A35" s="14" t="s">
+    <row r="37" spans="1:35" ht="24" customHeight="1">
+      <c r="A37" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B37" s="10" t="s">
         <v>742</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C37" s="10" t="s">
         <v>743</v>
       </c>
     </row>
-    <row r="36" spans="1:35" ht="24" customHeight="1">
-      <c r="B36" s="10" t="s">
+    <row r="38" spans="1:35" ht="24" customHeight="1">
+      <c r="B38" s="10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:35" ht="24" customHeight="1">
-      <c r="B37" s="11"/>
-      <c r="AA37" s="6" t="s">
+    <row r="39" spans="1:35" ht="24" customHeight="1">
+      <c r="B39" s="11" t="s">
+        <v>745</v>
+      </c>
+      <c r="AA39" s="6" t="s">
         <v>744</v>
       </c>
-      <c r="AB37" s="6" t="s">
+      <c r="AB39" s="6" t="s">
         <v>745</v>
       </c>
-      <c r="AC37" s="6" t="s">
+      <c r="AC39" s="6" t="s">
         <v>746</v>
       </c>
-      <c r="AD37" s="6" t="s">
+      <c r="AD39" s="6" t="s">
         <v>747</v>
       </c>
-      <c r="AE37" s="6" t="s">
+      <c r="AE39" s="6" t="s">
         <v>748</v>
       </c>
-      <c r="AF37" s="6" t="s">
+      <c r="AF39" s="6" t="s">
         <v>749</v>
       </c>
-      <c r="AG37" s="6" t="s">
+      <c r="AG39" s="6" t="s">
         <v>750</v>
       </c>
-      <c r="AH37" s="6" t="s">
+      <c r="AH39" s="6" t="s">
         <v>751</v>
       </c>
-      <c r="AI37" s="6" t="s">
+      <c r="AI39" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="1:35" ht="24" customHeight="1">
+      <c r="B40" s="11" t="s">
+        <v>746</v>
+      </c>
+      <c r="AA40" s="6" t="s">
+        <v>744</v>
+      </c>
+      <c r="AB40" s="6" t="s">
+        <v>745</v>
+      </c>
+      <c r="AC40" s="6" t="s">
+        <v>746</v>
+      </c>
+      <c r="AD40" s="6" t="s">
+        <v>747</v>
+      </c>
+      <c r="AE40" s="6" t="s">
+        <v>748</v>
+      </c>
+      <c r="AF40" s="6" t="s">
+        <v>749</v>
+      </c>
+      <c r="AG40" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="AH40" s="6" t="s">
+        <v>751</v>
+      </c>
+      <c r="AI40" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="1:35" ht="24" customHeight="1">
+      <c r="B41" s="11" t="s">
+        <v>747</v>
+      </c>
+      <c r="AA41" s="6" t="s">
+        <v>744</v>
+      </c>
+      <c r="AB41" s="6" t="s">
+        <v>745</v>
+      </c>
+      <c r="AC41" s="6" t="s">
+        <v>746</v>
+      </c>
+      <c r="AD41" s="6" t="s">
+        <v>747</v>
+      </c>
+      <c r="AE41" s="6" t="s">
+        <v>748</v>
+      </c>
+      <c r="AF41" s="6" t="s">
+        <v>749</v>
+      </c>
+      <c r="AG41" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="AH41" s="6" t="s">
+        <v>751</v>
+      </c>
+      <c r="AI41" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:35" ht="24" customHeight="1">
+      <c r="B42" s="11" t="s">
+        <v>748</v>
+      </c>
+      <c r="AA42" s="6" t="s">
+        <v>744</v>
+      </c>
+      <c r="AB42" s="6" t="s">
+        <v>745</v>
+      </c>
+      <c r="AC42" s="6" t="s">
+        <v>746</v>
+      </c>
+      <c r="AD42" s="6" t="s">
+        <v>747</v>
+      </c>
+      <c r="AE42" s="6" t="s">
+        <v>748</v>
+      </c>
+      <c r="AF42" s="6" t="s">
+        <v>749</v>
+      </c>
+      <c r="AG42" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="AH42" s="6" t="s">
+        <v>751</v>
+      </c>
+      <c r="AI42" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="1:35" ht="24" customHeight="1">
+      <c r="B43" s="11" t="s">
+        <v>749</v>
+      </c>
+      <c r="AA43" s="6" t="s">
+        <v>744</v>
+      </c>
+      <c r="AB43" s="6" t="s">
+        <v>745</v>
+      </c>
+      <c r="AC43" s="6" t="s">
+        <v>746</v>
+      </c>
+      <c r="AD43" s="6" t="s">
+        <v>747</v>
+      </c>
+      <c r="AE43" s="6" t="s">
+        <v>748</v>
+      </c>
+      <c r="AF43" s="6" t="s">
+        <v>749</v>
+      </c>
+      <c r="AG43" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="AH43" s="6" t="s">
+        <v>751</v>
+      </c>
+      <c r="AI43" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="1:35" ht="24" customHeight="1">
+      <c r="B44" s="11" t="s">
+        <v>750</v>
+      </c>
+      <c r="AA44" s="6" t="s">
+        <v>744</v>
+      </c>
+      <c r="AB44" s="6" t="s">
+        <v>745</v>
+      </c>
+      <c r="AC44" s="6" t="s">
+        <v>746</v>
+      </c>
+      <c r="AD44" s="6" t="s">
+        <v>747</v>
+      </c>
+      <c r="AE44" s="6" t="s">
+        <v>748</v>
+      </c>
+      <c r="AF44" s="6" t="s">
+        <v>749</v>
+      </c>
+      <c r="AG44" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="AH44" s="6" t="s">
+        <v>751</v>
+      </c>
+      <c r="AI44" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="1:35" ht="24" customHeight="1">
+      <c r="B45" s="11" t="s">
+        <v>751</v>
+      </c>
+      <c r="AA45" s="6" t="s">
+        <v>744</v>
+      </c>
+      <c r="AB45" s="6" t="s">
+        <v>745</v>
+      </c>
+      <c r="AC45" s="6" t="s">
+        <v>746</v>
+      </c>
+      <c r="AD45" s="6" t="s">
+        <v>747</v>
+      </c>
+      <c r="AE45" s="6" t="s">
+        <v>748</v>
+      </c>
+      <c r="AF45" s="6" t="s">
+        <v>749</v>
+      </c>
+      <c r="AG45" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="AH45" s="6" t="s">
+        <v>751</v>
+      </c>
+      <c r="AI45" s="6" t="s">
         <v>66</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="15"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24" xr:uid="{00000000-0002-0000-0700-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24:B26" xr:uid="{AD4C23DD-19E1-4052-9E29-AA7BF46E6507}">
       <formula1>AA24:AE24</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B37" xr:uid="{00000000-0002-0000-0700-000001000000}">
-      <formula1>AA37:AI37</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B39:B45" xr:uid="{957C4D8C-84BC-4B8C-B272-F5FCBD07CACC}">
+      <formula1>AA39:AI39</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10304,7 +11294,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AH89"/>
+  <dimension ref="A1:AH95"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -10376,7 +11366,9 @@
       </c>
     </row>
     <row r="11" spans="1:29" ht="178.05" customHeight="1">
-      <c r="B11" s="11"/>
+      <c r="B11" s="11" t="s">
+        <v>1102</v>
+      </c>
     </row>
     <row r="13" spans="1:29" ht="24" customHeight="1">
       <c r="A13" s="9" t="s">
@@ -10403,7 +11395,9 @@
       </c>
     </row>
     <row r="16" spans="1:29" ht="24" customHeight="1">
-      <c r="B16" s="11"/>
+      <c r="B16" s="11" t="s">
+        <v>1103</v>
+      </c>
       <c r="AA16" s="6" t="s">
         <v>764</v>
       </c>
@@ -10411,7 +11405,7 @@
         <v>765</v>
       </c>
       <c r="AC16" s="6" t="s">
-        <v>66</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="18" spans="1:34" ht="24" customHeight="1">
@@ -10434,7 +11428,9 @@
       </c>
     </row>
     <row r="20" spans="1:34" ht="24" customHeight="1">
-      <c r="B20" s="11"/>
+      <c r="B20" s="11" t="s">
+        <v>1105</v>
+      </c>
     </row>
     <row r="22" spans="1:34" ht="24" customHeight="1">
       <c r="A22" s="9" t="s">
@@ -10500,7 +11496,9 @@
       </c>
     </row>
     <row r="30" spans="1:34" ht="24" customHeight="1">
-      <c r="B30" s="11"/>
+      <c r="B30" s="11" t="s">
+        <v>778</v>
+      </c>
       <c r="AA30" s="6" t="s">
         <v>777</v>
       </c>
@@ -10526,387 +11524,574 @@
         <v>66</v>
       </c>
     </row>
+    <row r="31" spans="1:34" ht="24" customHeight="1">
+      <c r="B31" s="11" t="s">
+        <v>383</v>
+      </c>
+      <c r="AA31" s="6" t="s">
+        <v>777</v>
+      </c>
+      <c r="AB31" s="6" t="s">
+        <v>778</v>
+      </c>
+      <c r="AC31" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD31" s="6" t="s">
+        <v>779</v>
+      </c>
+      <c r="AE31" s="6" t="s">
+        <v>732</v>
+      </c>
+      <c r="AF31" s="6" t="s">
+        <v>518</v>
+      </c>
+      <c r="AG31" s="6" t="s">
+        <v>780</v>
+      </c>
+      <c r="AH31" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
     <row r="32" spans="1:34" ht="24" customHeight="1">
-      <c r="A32" s="9" t="s">
+      <c r="B32" s="11" t="s">
+        <v>779</v>
+      </c>
+      <c r="AA32" s="6" t="s">
+        <v>777</v>
+      </c>
+      <c r="AB32" s="6" t="s">
+        <v>778</v>
+      </c>
+      <c r="AC32" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD32" s="6" t="s">
+        <v>779</v>
+      </c>
+      <c r="AE32" s="6" t="s">
+        <v>732</v>
+      </c>
+      <c r="AF32" s="6" t="s">
+        <v>518</v>
+      </c>
+      <c r="AG32" s="6" t="s">
+        <v>780</v>
+      </c>
+      <c r="AH32" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:34" ht="24" customHeight="1">
+      <c r="B33" s="11" t="s">
+        <v>732</v>
+      </c>
+      <c r="AA33" s="6" t="s">
+        <v>777</v>
+      </c>
+      <c r="AB33" s="6" t="s">
+        <v>778</v>
+      </c>
+      <c r="AC33" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD33" s="6" t="s">
+        <v>779</v>
+      </c>
+      <c r="AE33" s="6" t="s">
+        <v>732</v>
+      </c>
+      <c r="AF33" s="6" t="s">
+        <v>518</v>
+      </c>
+      <c r="AG33" s="6" t="s">
+        <v>780</v>
+      </c>
+      <c r="AH33" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:34" ht="24" customHeight="1">
+      <c r="B34" s="11" t="s">
+        <v>734</v>
+      </c>
+      <c r="AA34" s="6" t="s">
+        <v>777</v>
+      </c>
+      <c r="AB34" s="6" t="s">
+        <v>778</v>
+      </c>
+      <c r="AC34" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD34" s="6" t="s">
+        <v>779</v>
+      </c>
+      <c r="AE34" s="6" t="s">
+        <v>732</v>
+      </c>
+      <c r="AF34" s="6" t="s">
+        <v>518</v>
+      </c>
+      <c r="AG34" s="6" t="s">
+        <v>780</v>
+      </c>
+      <c r="AH34" s="6" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:34" ht="24" customHeight="1">
+      <c r="A36" s="9" t="s">
         <v>781</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B36" s="9" t="s">
         <v>782</v>
       </c>
     </row>
-    <row r="33" spans="1:32" ht="24" customHeight="1">
-      <c r="A33" s="14" t="s">
+    <row r="37" spans="1:34" ht="24" customHeight="1">
+      <c r="A37" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B37" s="10" t="s">
         <v>783</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C37" s="10" t="s">
         <v>784</v>
       </c>
     </row>
-    <row r="34" spans="1:32" ht="24" customHeight="1">
-      <c r="B34" s="10" t="s">
+    <row r="38" spans="1:34" ht="24" customHeight="1">
+      <c r="B38" s="10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:32" ht="24" customHeight="1">
-      <c r="B35" s="11"/>
-      <c r="AA35" s="6" t="s">
+    <row r="39" spans="1:34" ht="24" customHeight="1">
+      <c r="B39" s="11" t="s">
         <v>785</v>
       </c>
-      <c r="AB35" s="6" t="s">
+      <c r="AA39" s="6" t="s">
+        <v>785</v>
+      </c>
+      <c r="AB39" s="6" t="s">
         <v>786</v>
       </c>
-      <c r="AC35" s="6" t="s">
+      <c r="AC39" s="6" t="s">
         <v>787</v>
       </c>
-      <c r="AD35" s="6" t="s">
+      <c r="AD39" s="6" t="s">
         <v>788</v>
       </c>
-      <c r="AE35" s="6" t="s">
+      <c r="AE39" s="6" t="s">
         <v>789</v>
       </c>
-      <c r="AF35" s="6" t="s">
+      <c r="AF39" s="6" t="s">
         <v>790</v>
       </c>
     </row>
-    <row r="38" spans="1:32" ht="24" customHeight="1">
-      <c r="A38" s="12" t="s">
+    <row r="40" spans="1:34" ht="24" customHeight="1">
+      <c r="B40" s="11" t="s">
+        <v>786</v>
+      </c>
+      <c r="AA40" s="6" t="s">
+        <v>785</v>
+      </c>
+      <c r="AB40" s="6" t="s">
+        <v>786</v>
+      </c>
+      <c r="AC40" s="6" t="s">
+        <v>787</v>
+      </c>
+      <c r="AD40" s="6" t="s">
+        <v>788</v>
+      </c>
+      <c r="AE40" s="6" t="s">
+        <v>789</v>
+      </c>
+      <c r="AF40" s="6" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="41" spans="1:34" ht="24" customHeight="1">
+      <c r="B41" s="11" t="s">
+        <v>1107</v>
+      </c>
+      <c r="AA41" s="6" t="s">
+        <v>785</v>
+      </c>
+      <c r="AB41" s="6" t="s">
+        <v>786</v>
+      </c>
+      <c r="AC41" s="6" t="s">
+        <v>787</v>
+      </c>
+      <c r="AD41" s="6" t="s">
+        <v>788</v>
+      </c>
+      <c r="AE41" s="6" t="s">
+        <v>789</v>
+      </c>
+      <c r="AF41" s="6" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="44" spans="1:34" ht="24" customHeight="1">
+      <c r="A44" s="12" t="s">
         <v>791</v>
       </c>
-      <c r="B38" s="12" t="s">
+      <c r="B44" s="12" t="s">
         <v>792</v>
       </c>
     </row>
-    <row r="39" spans="1:32" ht="24" customHeight="1">
-      <c r="B39" s="13" t="s">
+    <row r="45" spans="1:34" ht="24" customHeight="1">
+      <c r="B45" s="13" t="s">
         <v>793</v>
       </c>
     </row>
-    <row r="41" spans="1:32" ht="24" customHeight="1">
-      <c r="A41" s="9" t="s">
+    <row r="47" spans="1:34" ht="24" customHeight="1">
+      <c r="A47" s="9" t="s">
         <v>794</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B47" s="9" t="s">
         <v>795</v>
       </c>
     </row>
-    <row r="42" spans="1:32" ht="24" customHeight="1">
-      <c r="A42" s="14" t="s">
+    <row r="48" spans="1:34" ht="24" customHeight="1">
+      <c r="A48" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B48" s="10" t="s">
         <v>796</v>
       </c>
-      <c r="C42" s="10" t="s">
+      <c r="C48" s="10" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="43" spans="1:32" ht="24" customHeight="1">
-      <c r="B43" s="11"/>
-      <c r="AA43" s="6" t="s">
+    <row r="49" spans="1:31" ht="24" customHeight="1">
+      <c r="B49" s="11" t="s">
+        <v>1108</v>
+      </c>
+      <c r="AA49" s="6" t="s">
         <v>798</v>
       </c>
-      <c r="AB43" s="6" t="s">
+      <c r="AB49" s="6" t="s">
         <v>799</v>
       </c>
-      <c r="AC43" s="6" t="s">
+      <c r="AC49" s="6" t="s">
         <v>800</v>
       </c>
-      <c r="AD43" s="6" t="s">
+      <c r="AD49" s="6" t="s">
         <v>801</v>
       </c>
-      <c r="AE43" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="45" spans="1:32" ht="24" customHeight="1">
-      <c r="A45" s="9" t="s">
+      <c r="AE49" s="6" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="50" spans="1:31" ht="24" customHeight="1"/>
+    <row r="51" spans="1:31" ht="24" customHeight="1">
+      <c r="A51" s="9" t="s">
         <v>802</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B51" s="9" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="46" spans="1:32" ht="24" customHeight="1">
-      <c r="A46" s="14" t="s">
+    <row r="52" spans="1:31" ht="24" customHeight="1">
+      <c r="A52" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="B52" s="10" t="s">
         <v>803</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="C52" s="10" t="s">
         <v>804</v>
       </c>
     </row>
-    <row r="47" spans="1:32" ht="24" customHeight="1">
-      <c r="B47" s="11"/>
-    </row>
-    <row r="50" spans="1:28" ht="24" customHeight="1">
-      <c r="A50" s="12" t="s">
+    <row r="53" spans="1:31" ht="24" customHeight="1">
+      <c r="B53" s="11" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="54" spans="1:31" ht="24" customHeight="1"/>
+    <row r="55" spans="1:31" ht="24" customHeight="1"/>
+    <row r="56" spans="1:31" ht="24" customHeight="1">
+      <c r="A56" s="12" t="s">
         <v>805</v>
       </c>
-      <c r="B50" s="12" t="s">
+      <c r="B56" s="12" t="s">
         <v>806</v>
       </c>
     </row>
-    <row r="51" spans="1:28" ht="24" customHeight="1">
-      <c r="B51" s="13" t="s">
+    <row r="57" spans="1:31" ht="24" customHeight="1">
+      <c r="B57" s="13" t="s">
         <v>807</v>
       </c>
     </row>
-    <row r="53" spans="1:28" ht="24" customHeight="1">
-      <c r="A53" s="9" t="s">
+    <row r="58" spans="1:31" ht="24" customHeight="1"/>
+    <row r="59" spans="1:31" ht="24" customHeight="1">
+      <c r="A59" s="9" t="s">
         <v>808</v>
       </c>
-      <c r="B53" s="9" t="s">
+      <c r="B59" s="9" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="54" spans="1:28" ht="24" customHeight="1">
-      <c r="A54" s="14" t="s">
+    <row r="60" spans="1:31" ht="24" customHeight="1">
+      <c r="A60" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="B54" s="10" t="s">
+      <c r="B60" s="10" t="s">
         <v>809</v>
       </c>
-      <c r="C54" s="10" t="s">
+      <c r="C60" s="10" t="s">
         <v>810</v>
       </c>
     </row>
-    <row r="55" spans="1:28" ht="24" customHeight="1">
-      <c r="B55" s="11"/>
-      <c r="AA55" s="6" t="s">
+    <row r="61" spans="1:31" ht="24" customHeight="1">
+      <c r="B61" s="11"/>
+      <c r="AA61" s="6" t="s">
         <v>764</v>
       </c>
-      <c r="AB55" s="6" t="s">
+      <c r="AB61" s="6" t="s">
         <v>765</v>
       </c>
     </row>
-    <row r="57" spans="1:28" ht="24" customHeight="1">
-      <c r="A57" s="9" t="s">
+    <row r="62" spans="1:31" ht="24" customHeight="1"/>
+    <row r="63" spans="1:31" ht="24" customHeight="1">
+      <c r="A63" s="9" t="s">
         <v>811</v>
       </c>
-      <c r="B57" s="9" t="s">
+      <c r="B63" s="9" t="s">
         <v>812</v>
       </c>
     </row>
-    <row r="58" spans="1:28" ht="24" customHeight="1">
-      <c r="A58" s="14" t="s">
+    <row r="64" spans="1:31" ht="24" customHeight="1">
+      <c r="A64" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B58" s="10" t="s">
+      <c r="B64" s="10" t="s">
         <v>813</v>
       </c>
-      <c r="C58" s="10" t="s">
+      <c r="C64" s="10" t="s">
         <v>814</v>
       </c>
     </row>
-    <row r="59" spans="1:28" ht="24" customHeight="1">
-      <c r="B59" s="11"/>
-    </row>
-    <row r="61" spans="1:28" ht="24" customHeight="1">
-      <c r="A61" s="9" t="s">
+    <row r="65" spans="1:29" ht="24" customHeight="1">
+      <c r="B65" s="11" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="66" spans="1:29" ht="24" customHeight="1"/>
+    <row r="67" spans="1:29" ht="24" customHeight="1">
+      <c r="A67" s="9" t="s">
         <v>815</v>
       </c>
-      <c r="B61" s="9" t="s">
+      <c r="B67" s="9" t="s">
         <v>816</v>
       </c>
     </row>
-    <row r="62" spans="1:28" ht="24" customHeight="1">
-      <c r="A62" s="14" t="s">
+    <row r="68" spans="1:29" ht="24" customHeight="1">
+      <c r="A68" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B62" s="10" t="s">
+      <c r="B68" s="10" t="s">
         <v>817</v>
       </c>
-      <c r="C62" s="10" t="s">
+      <c r="C68" s="10" t="s">
         <v>818</v>
       </c>
     </row>
-    <row r="63" spans="1:28" ht="24" customHeight="1">
-      <c r="B63" s="11"/>
-    </row>
-    <row r="65" spans="1:29" ht="24" customHeight="1">
-      <c r="A65" s="9" t="s">
+    <row r="69" spans="1:29" ht="24" customHeight="1">
+      <c r="B69" s="11"/>
+    </row>
+    <row r="71" spans="1:29" ht="24" customHeight="1">
+      <c r="A71" s="9" t="s">
         <v>819</v>
       </c>
-      <c r="B65" s="9" t="s">
+      <c r="B71" s="9" t="s">
         <v>820</v>
       </c>
     </row>
-    <row r="66" spans="1:29" ht="24" customHeight="1">
-      <c r="A66" s="14" t="s">
+    <row r="72" spans="1:29" ht="24" customHeight="1">
+      <c r="A72" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="B66" s="10" t="s">
+      <c r="B72" s="10" t="s">
         <v>821</v>
       </c>
-      <c r="C66" s="10" t="s">
+      <c r="C72" s="10" t="s">
         <v>822</v>
       </c>
     </row>
-    <row r="67" spans="1:29" ht="24" customHeight="1">
-      <c r="B67" s="10" t="s">
+    <row r="73" spans="1:29" ht="24" customHeight="1">
+      <c r="B73" s="10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="68" spans="1:29" ht="24" customHeight="1">
-      <c r="B68" s="11"/>
-      <c r="AA68" s="6" t="s">
+    <row r="74" spans="1:29" ht="24" customHeight="1">
+      <c r="B74" s="11" t="s">
+        <v>825</v>
+      </c>
+      <c r="AA74" s="6" t="s">
         <v>823</v>
       </c>
-      <c r="AB68" s="6" t="s">
+      <c r="AB74" s="6" t="s">
         <v>824</v>
       </c>
-      <c r="AC68" s="6" t="s">
+      <c r="AC74" s="6" t="s">
         <v>825</v>
       </c>
     </row>
-    <row r="71" spans="1:29" ht="24" customHeight="1">
-      <c r="A71" s="12" t="s">
+    <row r="75" spans="1:29" ht="24" customHeight="1"/>
+    <row r="76" spans="1:29" ht="24" customHeight="1"/>
+    <row r="77" spans="1:29" ht="24" customHeight="1">
+      <c r="A77" s="12" t="s">
         <v>826</v>
       </c>
-      <c r="B71" s="12" t="s">
+      <c r="B77" s="12" t="s">
         <v>827</v>
       </c>
     </row>
-    <row r="72" spans="1:29" ht="24" customHeight="1">
-      <c r="B72" s="13" t="s">
+    <row r="78" spans="1:29" ht="24" customHeight="1">
+      <c r="B78" s="13" t="s">
         <v>828</v>
       </c>
     </row>
-    <row r="74" spans="1:29" ht="24" customHeight="1">
-      <c r="A74" s="9" t="s">
+    <row r="79" spans="1:29" ht="24" customHeight="1"/>
+    <row r="80" spans="1:29" ht="24" customHeight="1">
+      <c r="A80" s="9" t="s">
         <v>829</v>
       </c>
-      <c r="B74" s="9" t="s">
+      <c r="B80" s="9" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="75" spans="1:29" ht="24" customHeight="1">
-      <c r="A75" s="14" t="s">
+    <row r="81" spans="1:29" ht="24" customHeight="1">
+      <c r="A81" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="B75" s="10" t="s">
+      <c r="B81" s="10" t="s">
         <v>830</v>
       </c>
-      <c r="C75" s="10" t="s">
+      <c r="C81" s="10" t="s">
         <v>831</v>
       </c>
     </row>
-    <row r="76" spans="1:29" ht="24" customHeight="1">
-      <c r="B76" s="11"/>
-      <c r="AA76" s="6" t="s">
+    <row r="82" spans="1:29" ht="24" customHeight="1">
+      <c r="B82" s="11"/>
+      <c r="AA82" s="6" t="s">
         <v>764</v>
       </c>
-      <c r="AB76" s="6" t="s">
+      <c r="AB82" s="6" t="s">
         <v>765</v>
       </c>
     </row>
-    <row r="78" spans="1:29" ht="24" customHeight="1">
-      <c r="A78" s="9" t="s">
+    <row r="83" spans="1:29" ht="24" customHeight="1"/>
+    <row r="84" spans="1:29" ht="24" customHeight="1">
+      <c r="A84" s="9" t="s">
         <v>832</v>
       </c>
-      <c r="B78" s="9" t="s">
+      <c r="B84" s="9" t="s">
         <v>812</v>
       </c>
     </row>
-    <row r="79" spans="1:29" ht="24" customHeight="1">
-      <c r="A79" s="14" t="s">
+    <row r="85" spans="1:29" ht="24" customHeight="1">
+      <c r="A85" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B79" s="10" t="s">
+      <c r="B85" s="10" t="s">
         <v>833</v>
       </c>
-      <c r="C79" s="10" t="s">
+      <c r="C85" s="10" t="s">
         <v>834</v>
       </c>
     </row>
-    <row r="80" spans="1:29" ht="24" customHeight="1">
-      <c r="B80" s="11"/>
-    </row>
-    <row r="82" spans="1:29" ht="24" customHeight="1">
-      <c r="A82" s="9" t="s">
+    <row r="86" spans="1:29" ht="24" customHeight="1">
+      <c r="B86" s="11" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="87" spans="1:29" ht="24" customHeight="1"/>
+    <row r="88" spans="1:29" ht="24" customHeight="1">
+      <c r="A88" s="9" t="s">
         <v>835</v>
       </c>
-      <c r="B82" s="9" t="s">
+      <c r="B88" s="9" t="s">
         <v>816</v>
       </c>
     </row>
-    <row r="83" spans="1:29" ht="24" customHeight="1">
-      <c r="A83" s="14" t="s">
+    <row r="89" spans="1:29" ht="24" customHeight="1">
+      <c r="A89" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B83" s="10" t="s">
+      <c r="B89" s="10" t="s">
         <v>836</v>
       </c>
-      <c r="C83" s="10" t="s">
+      <c r="C89" s="10" t="s">
         <v>837</v>
       </c>
     </row>
-    <row r="84" spans="1:29" ht="24" customHeight="1">
-      <c r="B84" s="11"/>
-    </row>
-    <row r="86" spans="1:29" ht="24" customHeight="1">
-      <c r="A86" s="9" t="s">
+    <row r="90" spans="1:29" ht="24" customHeight="1">
+      <c r="B90" s="11"/>
+    </row>
+    <row r="92" spans="1:29" ht="24" customHeight="1">
+      <c r="A92" s="9" t="s">
         <v>838</v>
       </c>
-      <c r="B86" s="9" t="s">
+      <c r="B92" s="9" t="s">
         <v>820</v>
       </c>
     </row>
-    <row r="87" spans="1:29" ht="24" customHeight="1">
-      <c r="A87" s="14" t="s">
+    <row r="93" spans="1:29" ht="24" customHeight="1">
+      <c r="A93" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="B87" s="10" t="s">
+      <c r="B93" s="10" t="s">
         <v>839</v>
       </c>
-      <c r="C87" s="10" t="s">
+      <c r="C93" s="10" t="s">
         <v>840</v>
       </c>
     </row>
-    <row r="88" spans="1:29" ht="24" customHeight="1">
-      <c r="B88" s="10" t="s">
+    <row r="94" spans="1:29" ht="24" customHeight="1">
+      <c r="B94" s="10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="89" spans="1:29" ht="24" customHeight="1">
-      <c r="B89" s="11"/>
-      <c r="AA89" s="6" t="s">
+    <row r="95" spans="1:29" ht="24" customHeight="1">
+      <c r="B95" s="11" t="s">
+        <v>825</v>
+      </c>
+      <c r="AA95" s="6" t="s">
         <v>823</v>
       </c>
-      <c r="AB89" s="6" t="s">
+      <c r="AB95" s="6" t="s">
         <v>824</v>
       </c>
-      <c r="AC89" s="6" t="s">
+      <c r="AC95" s="6" t="s">
         <v>825</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="15"/>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16 B89 B68" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16 B95 B74" xr:uid="{7356F092-F1B7-46F8-8384-DB211D730C82}">
       <formula1>AA16:AC16</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B25" xr:uid="{00000000-0002-0000-0800-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B25" xr:uid="{003A1EAE-CB23-4FDD-B3F9-B033B296A31D}">
       <formula1>AA25:AD25</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B30" xr:uid="{00000000-0002-0000-0800-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B30:B34" xr:uid="{243BC0D7-CB69-4003-833B-90BC927FC040}">
       <formula1>AA30:AH30</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B35" xr:uid="{00000000-0002-0000-0800-000003000000}">
-      <formula1>AA35:AF35</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B39:B41" xr:uid="{B3A0ECF8-8F69-441D-86C9-F9F3E18C8418}">
+      <formula1>AA39:AF39</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B43" xr:uid="{00000000-0002-0000-0800-000004000000}">
-      <formula1>AA43:AE43</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B49" xr:uid="{566F5C4F-4A0F-499F-89DB-38180E383E79}">
+      <formula1>AA49:AE49</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B55 B76" xr:uid="{00000000-0002-0000-0800-000005000000}">
-      <formula1>AA55:AB55</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B61 B82" xr:uid="{04F9980B-D52D-491E-AF3C-EA46B99C3793}">
+      <formula1>AA61:AB61</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B63 B84" xr:uid="{00000000-0002-0000-0800-000006000000}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B69 B90" xr:uid="{540D4D95-643D-42D3-8832-37A29FD87456}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>